<commit_message>
Edits to L05 on Program Families
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Work/Teaching/CAS741/2017/GradeCalculation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="2680" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="2920" yWindow="1900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -108,13 +103,22 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>https://github.com/aschaap/cas741.git</t>
+  </si>
+  <si>
+    <t>https://github.com/sccdsyad8663/Shusheng-CAS741.git</t>
+  </si>
+  <si>
+    <t>https://github.com/keshavd/cas741.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +160,22 @@
       <color theme="1"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,8 +210,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -204,7 +238,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -260,7 +308,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -295,7 +343,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -472,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -483,15 +531,15 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -516,7 +564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -530,12 +578,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="13" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -543,12 +594,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -556,7 +613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -567,46 +624,66 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to list of completed problem statements
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="2920" yWindow="1900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
@@ -11,18 +16,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -520,7 +525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -531,15 +536,15 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +558,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -564,7 +569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -578,7 +583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13" customHeight="1">
+    <row r="4" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -586,15 +591,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17" customHeight="1">
+    <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -605,15 +613,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -624,7 +635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -635,15 +646,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -654,7 +668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -665,7 +679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -680,10 +694,5 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to stdnt Repo list
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2920" yWindow="0" windowWidth="25600" windowHeight="27220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -525,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,16 +530,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -569,7 +567,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -583,7 +581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="13" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -591,18 +589,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="17" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -613,18 +608,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="J7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -635,7 +627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -646,18 +638,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="J10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -668,7 +657,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -679,7 +668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -694,5 +683,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Additional examples, revise blank project template, v and v lecture
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="0" windowWidth="25600" windowHeight="27220" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="38260" windowHeight="20280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Ma,Xiaoye (Marshall)</t>
   </si>
   <si>
-    <t>Problem Statement Approved</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -112,6 +109,18 @@
   </si>
   <si>
     <t>https://github.com/keshavd/cas741.git</t>
+  </si>
+  <si>
+    <t>Prob State</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Approved</t>
+  </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>REVIEWED BY THE PERSON LISTED BELOW</t>
   </si>
 </sst>
 </file>
@@ -210,8 +219,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -238,7 +251,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -246,6 +259,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -253,6 +268,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -528,17 +545,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.33203125" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -552,131 +569,202 @@
       <c r="G1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="J1" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="str">
+        <f>A4</f>
+        <v>Bicket,Isobel Claire</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="13" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="str">
+        <f>A5</f>
+        <v>Dial,Keshav</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="13" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="str">
+        <f>A6</f>
+        <v>Guttapati,Devi Prasad Reddy</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="str">
+        <f>A7</f>
+        <v>Li,Shusheng</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="str">
+        <f>A8</f>
+        <v>Ma,Xiaoye (Marshall)</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="str">
+        <f>A9</f>
+        <v>Palmer,Steven</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="str">
+        <f>A10</f>
+        <v>Pofelski,Alexandre</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="str">
+        <f>A11</f>
+        <v>Schaap,Alexander</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" t="s">
         <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="str">
+        <f>A12</f>
+        <v>Smith,Geneva Marie</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="str">
+        <f>A13</f>
+        <v>Zhang,Jason (Renjie)</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" t="str">
+        <f>A14</f>
+        <v>Zhao,Yuzhi</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="J13" t="s">
-        <v>26</v>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="str">
+        <f>A3</f>
+        <v>Aoanan,Paul Vincent Seva</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test plan template and repos.xlsx
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="38260" windowHeight="20280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32800" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -537,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,7 +548,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -598,7 +598,7 @@
         <v>25</v>
       </c>
       <c r="J3" t="str">
-        <f>A4</f>
+        <f t="shared" ref="J3:J13" si="0">A4</f>
         <v>Bicket,Isobel Claire</v>
       </c>
     </row>
@@ -616,7 +616,7 @@
         <v>25</v>
       </c>
       <c r="J4" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>Dial,Keshav</v>
       </c>
     </row>
@@ -627,8 +627,11 @@
       <c r="B5" t="s">
         <v>28</v>
       </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
       <c r="J5" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>Guttapati,Devi Prasad Reddy</v>
       </c>
     </row>
@@ -643,7 +646,7 @@
         <v>25</v>
       </c>
       <c r="J6" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>Li,Shusheng</v>
       </c>
     </row>
@@ -658,7 +661,7 @@
         <v>25</v>
       </c>
       <c r="J7" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>Ma,Xiaoye (Marshall)</v>
       </c>
     </row>
@@ -673,7 +676,7 @@
         <v>25</v>
       </c>
       <c r="J8" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>Palmer,Steven</v>
       </c>
     </row>
@@ -688,7 +691,7 @@
         <v>25</v>
       </c>
       <c r="J9" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>Pofelski,Alexandre</v>
       </c>
     </row>
@@ -703,7 +706,7 @@
         <v>25</v>
       </c>
       <c r="J10" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>Schaap,Alexander</v>
       </c>
     </row>
@@ -718,7 +721,7 @@
         <v>25</v>
       </c>
       <c r="J11" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>Smith,Geneva Marie</v>
       </c>
     </row>
@@ -733,7 +736,7 @@
         <v>25</v>
       </c>
       <c r="J12" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>Zhang,Jason (Renjie)</v>
       </c>
     </row>
@@ -748,7 +751,7 @@
         <v>25</v>
       </c>
       <c r="J13" t="str">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>Zhao,Yuzhi</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Addition of citations related to metamorphic testing
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32800" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -537,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,10 +553,10 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.33203125" customWidth="1"/>
@@ -559,7 +564,7 @@
     <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
       <c r="G2" s="3"/>
@@ -587,7 +592,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -602,7 +607,7 @@
         <v>Bicket,Isobel Claire</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -620,7 +625,7 @@
         <v>Dial,Keshav</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13" customHeight="1">
+    <row r="5" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -635,7 +640,7 @@
         <v>Guttapati,Devi Prasad Reddy</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" customHeight="1">
+    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -650,7 +655,7 @@
         <v>Li,Shusheng</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -665,7 +670,7 @@
         <v>Ma,Xiaoye (Marshall)</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -680,7 +685,7 @@
         <v>Palmer,Steven</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -695,7 +700,7 @@
         <v>Pofelski,Alexandre</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -710,7 +715,7 @@
         <v>Schaap,Alexander</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -725,7 +730,7 @@
         <v>Smith,Geneva Marie</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -740,7 +745,7 @@
         <v>Zhang,Jason (Renjie)</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -755,7 +760,7 @@
         <v>Zhao,Yuzhi</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -774,10 +779,5 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of VnV feedback partners to Repos.xlsx file
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="47520" windowHeight="21560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>REVIEWED BY THE PERSON LISTED BELOW</t>
+  </si>
+  <si>
+    <t>VnV Plan</t>
   </si>
 </sst>
 </file>
@@ -550,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,9 +565,10 @@
     <col min="6" max="6" width="3.33203125" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
       <c r="G2" s="3"/>
@@ -591,8 +595,11 @@
       <c r="J2" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -606,8 +613,12 @@
         <f t="shared" ref="J3:J13" si="0">A4</f>
         <v>Bicket,Isobel Claire</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" t="str">
+        <f>J4</f>
+        <v>Dial,Keshav</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -624,8 +635,12 @@
         <f t="shared" si="0"/>
         <v>Dial,Keshav</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" t="str">
+        <f>J5</f>
+        <v>Guttapati,Devi Prasad Reddy</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -639,8 +654,12 @@
         <f t="shared" si="0"/>
         <v>Guttapati,Devi Prasad Reddy</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5" t="str">
+        <f>J6</f>
+        <v>Li,Shusheng</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -654,8 +673,12 @@
         <f t="shared" si="0"/>
         <v>Li,Shusheng</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" t="str">
+        <f>J7</f>
+        <v>Ma,Xiaoye (Marshall)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -669,8 +692,12 @@
         <f t="shared" si="0"/>
         <v>Ma,Xiaoye (Marshall)</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" t="str">
+        <f>J8</f>
+        <v>Palmer,Steven</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -684,8 +711,12 @@
         <f t="shared" si="0"/>
         <v>Palmer,Steven</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" t="str">
+        <f>J9</f>
+        <v>Pofelski,Alexandre</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -699,8 +730,12 @@
         <f t="shared" si="0"/>
         <v>Pofelski,Alexandre</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" t="str">
+        <f>J10</f>
+        <v>Schaap,Alexander</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -714,8 +749,12 @@
         <f t="shared" si="0"/>
         <v>Schaap,Alexander</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" t="str">
+        <f>J11</f>
+        <v>Smith,Geneva Marie</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -729,8 +768,12 @@
         <f t="shared" si="0"/>
         <v>Smith,Geneva Marie</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" t="str">
+        <f>J12</f>
+        <v>Zhang,Jason (Renjie)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -744,8 +787,12 @@
         <f t="shared" si="0"/>
         <v>Zhang,Jason (Renjie)</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" t="str">
+        <f>J13</f>
+        <v>Zhao,Yuzhi</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -759,8 +806,12 @@
         <f t="shared" si="0"/>
         <v>Zhao,Yuzhi</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" t="str">
+        <f>J14</f>
+        <v>Aoanan,Paul Vincent Seva</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -773,6 +824,10 @@
       <c r="J14" t="str">
         <f>A3</f>
         <v>Aoanan,Paul Vincent Seva</v>
+      </c>
+      <c r="K14" t="str">
+        <f>J3</f>
+        <v>Bicket,Isobel Claire</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to repos file to reflect partners for remaining deliverables.
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="47520" windowHeight="21560" tabRatio="500"/>
+    <workbookView xWindow="1580" yWindow="1720" windowWidth="47520" windowHeight="21560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>VnV Plan</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>MIS</t>
   </si>
 </sst>
 </file>
@@ -227,8 +233,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -259,7 +269,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -269,6 +279,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -278,6 +290,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,10 +579,12 @@
     <col min="6" max="6" width="3.33203125" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.5" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
       <c r="G2" s="3"/>
@@ -598,8 +614,14 @@
       <c r="K2" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -614,11 +636,19 @@
         <v>Bicket,Isobel Claire</v>
       </c>
       <c r="K3" t="str">
-        <f>J4</f>
+        <f t="shared" ref="K3:M14" si="1">J4</f>
         <v>Dial,Keshav</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="str">
+        <f t="shared" si="1"/>
+        <v>Guttapati,Devi Prasad Reddy</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="1"/>
+        <v>Li,Shusheng</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -636,11 +666,19 @@
         <v>Dial,Keshav</v>
       </c>
       <c r="K4" t="str">
-        <f>J5</f>
+        <f t="shared" si="1"/>
         <v>Guttapati,Devi Prasad Reddy</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>Li,Shusheng</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>Ma,Xiaoye (Marshall)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -655,11 +693,19 @@
         <v>Guttapati,Devi Prasad Reddy</v>
       </c>
       <c r="K5" t="str">
-        <f>J6</f>
+        <f t="shared" si="1"/>
         <v>Li,Shusheng</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>Ma,Xiaoye (Marshall)</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>Palmer,Steven</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -674,11 +720,19 @@
         <v>Li,Shusheng</v>
       </c>
       <c r="K6" t="str">
-        <f>J7</f>
+        <f t="shared" si="1"/>
         <v>Ma,Xiaoye (Marshall)</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>Palmer,Steven</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>Pofelski,Alexandre</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -693,11 +747,19 @@
         <v>Ma,Xiaoye (Marshall)</v>
       </c>
       <c r="K7" t="str">
-        <f>J8</f>
+        <f t="shared" si="1"/>
         <v>Palmer,Steven</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
+        <v>Pofelski,Alexandre</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>Schaap,Alexander</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -712,11 +774,19 @@
         <v>Palmer,Steven</v>
       </c>
       <c r="K8" t="str">
-        <f>J9</f>
+        <f t="shared" si="1"/>
         <v>Pofelski,Alexandre</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
+        <v>Schaap,Alexander</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>Smith,Geneva Marie</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -731,11 +801,19 @@
         <v>Pofelski,Alexandre</v>
       </c>
       <c r="K9" t="str">
-        <f>J10</f>
+        <f t="shared" si="1"/>
         <v>Schaap,Alexander</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>Smith,Geneva Marie</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>Zhang,Jason (Renjie)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -750,11 +828,19 @@
         <v>Schaap,Alexander</v>
       </c>
       <c r="K10" t="str">
-        <f>J11</f>
+        <f t="shared" si="1"/>
         <v>Smith,Geneva Marie</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>Zhang,Jason (Renjie)</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>Zhao,Yuzhi</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -769,11 +855,19 @@
         <v>Smith,Geneva Marie</v>
       </c>
       <c r="K11" t="str">
-        <f>J12</f>
+        <f t="shared" si="1"/>
         <v>Zhang,Jason (Renjie)</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
+        <v>Zhao,Yuzhi</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>Aoanan,Paul Vincent Seva</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -788,11 +882,19 @@
         <v>Zhang,Jason (Renjie)</v>
       </c>
       <c r="K12" t="str">
-        <f>J13</f>
+        <f t="shared" si="1"/>
         <v>Zhao,Yuzhi</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" t="str">
+        <f t="shared" si="1"/>
+        <v>Aoanan,Paul Vincent Seva</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>Bicket,Isobel Claire</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -807,11 +909,19 @@
         <v>Zhao,Yuzhi</v>
       </c>
       <c r="K13" t="str">
-        <f>J14</f>
+        <f t="shared" si="1"/>
         <v>Aoanan,Paul Vincent Seva</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" t="str">
+        <f t="shared" si="1"/>
+        <v>Bicket,Isobel Claire</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>Dial,Keshav</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -828,6 +938,14 @@
       <c r="K14" t="str">
         <f>J3</f>
         <v>Bicket,Isobel Claire</v>
+      </c>
+      <c r="L14" t="str">
+        <f>K3</f>
+        <v>Dial,Keshav</v>
+      </c>
+      <c r="M14" t="str">
+        <f>L3</f>
+        <v>Guttapati,Devi Prasad Reddy</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mention of GitHub review of colleagues implementation
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>MIS</t>
+  </si>
+  <si>
+    <t>Implement</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,9 +585,10 @@
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
     <col min="11" max="11" width="25.5" customWidth="1"/>
     <col min="12" max="12" width="24.83203125" customWidth="1"/>
+    <col min="13" max="13" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +605,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
       <c r="G2" s="3"/>
@@ -620,8 +624,11 @@
       <c r="M2" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -636,7 +643,7 @@
         <v>Bicket,Isobel Claire</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:M14" si="1">J4</f>
+        <f t="shared" ref="K3:N13" si="1">J4</f>
         <v>Dial,Keshav</v>
       </c>
       <c r="L3" t="str">
@@ -647,8 +654,12 @@
         <f t="shared" si="1"/>
         <v>Li,Shusheng</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="str">
+        <f t="shared" si="1"/>
+        <v>Ma,Xiaoye (Marshall)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -677,8 +688,12 @@
         <f t="shared" si="1"/>
         <v>Ma,Xiaoye (Marshall)</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N4" t="str">
+        <f t="shared" si="1"/>
+        <v>Palmer,Steven</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -704,8 +719,12 @@
         <f t="shared" si="1"/>
         <v>Palmer,Steven</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>Pofelski,Alexandre</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -731,8 +750,12 @@
         <f t="shared" si="1"/>
         <v>Pofelski,Alexandre</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>Schaap,Alexander</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -758,8 +781,12 @@
         <f t="shared" si="1"/>
         <v>Schaap,Alexander</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="str">
+        <f t="shared" si="1"/>
+        <v>Smith,Geneva Marie</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -785,8 +812,12 @@
         <f t="shared" si="1"/>
         <v>Smith,Geneva Marie</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="str">
+        <f t="shared" si="1"/>
+        <v>Zhang,Jason (Renjie)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -812,8 +843,12 @@
         <f t="shared" si="1"/>
         <v>Zhang,Jason (Renjie)</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="str">
+        <f t="shared" si="1"/>
+        <v>Zhao,Yuzhi</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -839,8 +874,12 @@
         <f t="shared" si="1"/>
         <v>Zhao,Yuzhi</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>Aoanan,Paul Vincent Seva</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -866,8 +905,12 @@
         <f t="shared" si="1"/>
         <v>Aoanan,Paul Vincent Seva</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>Bicket,Isobel Claire</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -893,8 +936,12 @@
         <f t="shared" si="1"/>
         <v>Bicket,Isobel Claire</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="str">
+        <f t="shared" si="1"/>
+        <v>Dial,Keshav</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -920,8 +967,12 @@
         <f t="shared" si="1"/>
         <v>Dial,Keshav</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" t="str">
+        <f t="shared" si="1"/>
+        <v>Guttapati,Devi Prasad Reddy</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -946,6 +997,10 @@
       <c r="M14" t="str">
         <f>L3</f>
         <v>Guttapati,Devi Prasad Reddy</v>
+      </c>
+      <c r="N14" t="str">
+        <f>M3</f>
+        <v>Li,Shusheng</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to list of projects
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75630923-7359-984F-AABA-E5EC4C9C761E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80349B65-CE8B-8A4D-AB7B-FE4BDCEE18E5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1720" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17380" yWindow="2460" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$13</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -78,16 +78,46 @@
     <t>Owojaiye, Oluwaseun</t>
   </si>
   <si>
-    <t>Wang, Yu</t>
-  </si>
-  <si>
     <t>White, Robert</t>
   </si>
   <si>
     <t>Zlitni, Hanane</t>
   </si>
   <si>
-    <t>Malavika Srinivasan</t>
+    <t>https://github.com/hananezlitni/HZ-CAS741-Project</t>
+  </si>
+  <si>
+    <t>https://github.com/PeaWagon/Kaplan</t>
+  </si>
+  <si>
+    <t>https://github.com/whitere123/CAS741_REW</t>
+  </si>
+  <si>
+    <t>https://github.com/Malavika-Srinivasan/CAS741</t>
+  </si>
+  <si>
+    <t>https://github.com/smiths/caseStudies/tree/master/CaseStudies/ssp</t>
+  </si>
+  <si>
+    <t>https://github.com/smiths/caseStudies/tree/master/CaseStudies/glass</t>
+  </si>
+  <si>
+    <t>https://github.com/smiths/caseStudies/tree/master/CaseStudies/gamephys</t>
+  </si>
+  <si>
+    <t>Lu, Yang</t>
+  </si>
+  <si>
+    <t>Sekis, Karol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srinivasan, Malavika </t>
+  </si>
+  <si>
+    <t>Wu, Qirui</t>
+  </si>
+  <si>
+    <t>Zhang, Jian</t>
   </si>
 </sst>
 </file>
@@ -598,16 +628,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
@@ -668,362 +698,297 @@
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="str">
-        <f>A4</f>
+        <f>A5</f>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="G3" s="8" t="str">
-        <f t="shared" ref="G3:J13" si="0">F4</f>
+        <f>F5</f>
         <v>Motamer, Vajiheh</v>
       </c>
       <c r="H3" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>G5</f>
         <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="I3" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Wang, Yu</v>
+        <f>H5</f>
+        <v>Sekis, Karol</v>
       </c>
       <c r="J3" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f>I5</f>
         <v>White, Robert</v>
       </c>
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="8" t="str">
-        <f>A5</f>
-        <v>Motamer, Vajiheh</v>
-      </c>
-      <c r="G4" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Owojaiye, Oluwaseun</v>
-      </c>
-      <c r="H4" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Wang, Yu</v>
-      </c>
-      <c r="I4" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>White, Robert</v>
-      </c>
-      <c r="J4" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Zlitni, Hanane</v>
-      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="str">
-        <f>A6</f>
+        <f t="shared" ref="F5:F7" si="0">A6</f>
+        <v>Motamer, Vajiheh</v>
+      </c>
+      <c r="G5" s="8" t="str">
+        <f t="shared" ref="G5:J7" si="1">F6</f>
         <v>Owojaiye, Oluwaseun</v>
       </c>
-      <c r="G5" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Wang, Yu</v>
-      </c>
       <c r="H5" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>Sekis, Karol</v>
+      </c>
+      <c r="I5" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>White, Robert</v>
       </c>
-      <c r="I5" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="J5" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Zlitni, Hanane</v>
       </c>
-      <c r="J5" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Malavika Srinivasan</v>
-      </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="str">
-        <f>A7</f>
-        <v>Wang, Yu</v>
+        <f t="shared" si="0"/>
+        <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="G6" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>Sekis, Karol</v>
+      </c>
+      <c r="H6" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>White, Robert</v>
       </c>
-      <c r="H6" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="I6" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Zlitni, Hanane</v>
       </c>
-      <c r="I6" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Malavika Srinivasan</v>
-      </c>
-      <c r="J6" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="J6" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
+        <v>Sekis, Karol</v>
+      </c>
+      <c r="G7" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>White, Robert</v>
       </c>
-      <c r="G7" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="H7" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Zlitni, Hanane</v>
       </c>
-      <c r="H7" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Malavika Srinivasan</v>
-      </c>
-      <c r="I7" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="I7" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J7" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
       </c>
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="str">
-        <f>A9</f>
+        <f>A10</f>
+        <v>White, Robert</v>
+      </c>
+      <c r="G8" s="8" t="str">
+        <f>F10</f>
         <v>Zlitni, Hanane</v>
       </c>
-      <c r="G8" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Malavika Srinivasan</v>
-      </c>
-      <c r="H8" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H8" s="8" t="e">
+        <f>G10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I8" s="8" t="e">
+        <f>H10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J8" s="8" t="e">
+        <f>I10</f>
+        <v>#REF!</v>
       </c>
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="8" t="str">
-        <f>A10</f>
-        <v>Malavika Srinivasan</v>
-      </c>
-      <c r="G9" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="8">
-        <f>A11</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Garner, Jennifer</v>
+      <c r="F10" s="8" t="str">
+        <f>A13</f>
+        <v>Zlitni, Hanane</v>
+      </c>
+      <c r="G10" s="8" t="e">
+        <f>F13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H10" s="8" t="e">
+        <f>G13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I10" s="8" t="e">
+        <f>H13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J10" s="8" t="e">
+        <f>I13</f>
+        <v>#REF!</v>
       </c>
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="11"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="8">
-        <f>A12</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="J11" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>MacLachlan, Brooks</v>
-      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="11"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="8">
-        <f>A13</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="I12" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="J12" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Motamer, Vajiheh</v>
-      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="8">
-        <f>A14</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="H13" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="I13" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Motamer, Vajiheh</v>
-      </c>
-      <c r="J13" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Owojaiye, Oluwaseun</v>
+      <c r="F13" s="8" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G13" s="8" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H13" s="8" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I13" s="8" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" s="8" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="str">
-        <f>A3</f>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="G14" s="8" t="str">
-        <f>F3</f>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="H14" s="8" t="str">
-        <f>G3</f>
-        <v>Motamer, Vajiheh</v>
-      </c>
-      <c r="I14" s="8" t="str">
-        <f>H3</f>
-        <v>Owojaiye, Oluwaseun</v>
-      </c>
-      <c r="J14" s="8" t="str">
-        <f>I3</f>
-        <v>Wang, Yu</v>
-      </c>
-      <c r="K14" s="10"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{8860323E-E796-6542-9DBE-B172243EFBE2}"/>
+  </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
Approved Brooks's problem statement
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80349B65-CE8B-8A4D-AB7B-FE4BDCEE18E5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0450D2-D720-674D-9BE7-F12914944419}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17380" yWindow="2460" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13120" yWindow="1420" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$13</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Zhang, Jian</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -631,14 +634,15 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="62.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
@@ -749,7 +753,9 @@
         <v>21</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="str">
         <f t="shared" ref="F5:F7" si="0">A6</f>

</xml_diff>

<commit_message>
Updates to reference list, repo list
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0450D2-D720-674D-9BE7-F12914944419}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FFF2E3-C2C6-514C-BDBE-D53F64214B23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13120" yWindow="1420" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -634,7 +634,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,7 +960,9 @@
         <v>17</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="e">
         <f>#REF!</f>

</xml_diff>

<commit_message>
Edit to this years list of student repos
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FFF2E3-C2C6-514C-BDBE-D53F64214B23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044F8DF0-F253-3547-AEAD-A0238A0459EC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13120" yWindow="1420" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$13</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -634,7 +634,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,7 +706,9 @@
         <v>18</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="str">
         <f>A5</f>

</xml_diff>

<commit_message>
Updates to repo list
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044F8DF0-F253-3547-AEAD-A0238A0459EC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134D2698-CE40-9047-A689-7380B407DF7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13120" yWindow="1420" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$11</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -105,9 +105,6 @@
     <t>https://github.com/smiths/caseStudies/tree/master/CaseStudies/gamephys</t>
   </si>
   <si>
-    <t>Lu, Yang</t>
-  </si>
-  <si>
     <t>Sekis, Karol</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
   </si>
   <si>
     <t>Wu, Qirui</t>
-  </si>
-  <si>
-    <t>Zhang, Jian</t>
   </si>
   <si>
     <t>YES</t>
@@ -631,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,140 +701,155 @@
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="str">
-        <f>A5</f>
+        <f>A4</f>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="G3" s="8" t="str">
-        <f>F5</f>
+        <f>F4</f>
         <v>Motamer, Vajiheh</v>
       </c>
       <c r="H3" s="8" t="str">
-        <f>G5</f>
+        <f>G4</f>
         <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="I3" s="8" t="str">
-        <f>H5</f>
+        <f>H4</f>
         <v>Sekis, Karol</v>
       </c>
       <c r="J3" s="8" t="str">
-        <f>I5</f>
-        <v>White, Robert</v>
+        <f>I4</f>
+        <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="F4" s="8" t="str">
+        <f>A5</f>
+        <v>Motamer, Vajiheh</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f>F5</f>
+        <v>Owojaiye, Oluwaseun</v>
+      </c>
+      <c r="H4" s="8" t="str">
+        <f t="shared" ref="G4:J6" si="0">G5</f>
+        <v>Sekis, Karol</v>
+      </c>
+      <c r="I4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Srinivasan, Malavika </v>
+      </c>
+      <c r="J4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>White, Robert</v>
+      </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="8" t="s">
-        <v>29</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="str">
-        <f t="shared" ref="F5:F7" si="0">A6</f>
-        <v>Motamer, Vajiheh</v>
+        <f>A6</f>
+        <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="G5" s="8" t="str">
-        <f t="shared" ref="G5:J7" si="1">F6</f>
-        <v>Owojaiye, Oluwaseun</v>
+        <f>F6</f>
+        <v>Sekis, Karol</v>
       </c>
       <c r="H5" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Sekis, Karol</v>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="I5" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>White, Robert</v>
       </c>
       <c r="J5" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="str">
+        <f>A7</f>
+        <v>Sekis, Karol</v>
+      </c>
+      <c r="G6" s="8" t="str">
+        <f>F7</f>
+        <v xml:space="preserve">Srinivasan, Malavika </v>
+      </c>
+      <c r="H6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Owojaiye, Oluwaseun</v>
-      </c>
-      <c r="G6" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Sekis, Karol</v>
-      </c>
-      <c r="H6" s="8" t="str">
-        <f t="shared" si="1"/>
         <v>White, Robert</v>
       </c>
       <c r="I6" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Zlitni, Hanane</v>
       </c>
-      <c r="J6" s="8" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="J6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>MacLachlan, Brooks</v>
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Sekis, Karol</v>
+        <f>A8</f>
+        <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="G7" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f>F8</f>
         <v>White, Robert</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f>G9</f>
         <v>Zlitni, Hanane</v>
       </c>
-      <c r="I7" s="8" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
+      <c r="I7" s="8" t="str">
+        <f>H9</f>
+        <v>MacLachlan, Brooks</v>
       </c>
       <c r="J7" s="8" t="e">
-        <f t="shared" si="1"/>
+        <f>I9</f>
         <v>#REF!</v>
       </c>
       <c r="K7" s="10"/>
@@ -849,155 +858,122 @@
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="str">
-        <f>A10</f>
+        <f>A9</f>
         <v>White, Robert</v>
       </c>
       <c r="G8" s="8" t="str">
-        <f>F10</f>
-        <v>Zlitni, Hanane</v>
-      </c>
-      <c r="H8" s="8" t="e">
-        <f>G10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I8" s="8" t="e">
-        <f>H10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J8" s="8" t="e">
-        <f>I10</f>
-        <v>#REF!</v>
-      </c>
+        <f>F9</f>
+        <v>Wu, Qirui</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="F9" s="8" t="str">
+        <f>A10</f>
+        <v>Wu, Qirui</v>
+      </c>
+      <c r="G9" s="8" t="str">
+        <f>F10</f>
+        <v>Zlitni, Hanane</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f>G11</f>
+        <v>MacLachlan, Brooks</v>
+      </c>
+      <c r="I9" s="8" t="e">
+        <f>H11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" s="8" t="e">
+        <f>I11</f>
+        <v>#REF!</v>
+      </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>19</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B10" s="11"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="str">
-        <f>A13</f>
+        <f>A11</f>
         <v>Zlitni, Hanane</v>
       </c>
-      <c r="G10" s="8" t="e">
-        <f>F13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H10" s="8" t="e">
-        <f>G13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I10" s="8" t="e">
-        <f>H13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J10" s="8" t="e">
-        <f>I13</f>
-        <v>#REF!</v>
-      </c>
+      <c r="G10" s="8" t="str">
+        <f>F11</f>
+        <v>Garner, Jennifer</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="e">
+      <c r="F11" s="8" t="str">
+        <f>A3</f>
+        <v>Garner, Jennifer</v>
+      </c>
+      <c r="G11" s="8" t="str">
+        <f>F3</f>
+        <v>MacLachlan, Brooks</v>
+      </c>
+      <c r="H11" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G13" s="8" t="e">
+      <c r="I11" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="H13" s="8" t="e">
+      <c r="J11" s="8" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="I13" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{8860323E-E796-6542-9DBE-B172243EFBE2}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{8860323E-E796-6542-9DBE-B172243EFBE2}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Robert Prob. Statement approved.
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134D2698-CE40-9047-A689-7380B407DF7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23124D4-9983-284C-B1EE-47BA5F36787C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13120" yWindow="1420" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,7 +705,7 @@
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="str">
-        <f>A4</f>
+        <f t="shared" ref="F3:F10" si="0">A4</f>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="G3" s="8" t="str">
@@ -739,23 +739,23 @@
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>Motamer, Vajiheh</v>
       </c>
       <c r="G4" s="8" t="str">
-        <f>F5</f>
+        <f t="shared" ref="G4:G10" si="1">F5</f>
         <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="H4" s="8" t="str">
-        <f t="shared" ref="G4:J6" si="0">G5</f>
+        <f t="shared" ref="H4:J6" si="2">G5</f>
         <v>Sekis, Karol</v>
       </c>
       <c r="I4" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="J4" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>White, Robert</v>
       </c>
       <c r="K4" s="10"/>
@@ -771,23 +771,23 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="G5" s="8" t="str">
-        <f>F6</f>
+        <f t="shared" si="1"/>
         <v>Sekis, Karol</v>
       </c>
       <c r="H5" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="I5" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>White, Robert</v>
       </c>
       <c r="J5" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="K5" s="10"/>
@@ -803,23 +803,23 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>Sekis, Karol</v>
       </c>
       <c r="G6" s="8" t="str">
-        <f>F7</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="H6" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>White, Robert</v>
       </c>
       <c r="I6" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="J6" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="K6" s="10"/>
@@ -833,11 +833,11 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>F8</f>
+        <f t="shared" si="1"/>
         <v>White, Robert</v>
       </c>
       <c r="H7" s="8" t="str">
@@ -865,11 +865,11 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>White, Robert</v>
       </c>
       <c r="G8" s="8" t="str">
-        <f>F9</f>
+        <f t="shared" si="1"/>
         <v>Wu, Qirui</v>
       </c>
       <c r="H8" s="8"/>
@@ -885,14 +885,16 @@
         <v>19</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>Wu, Qirui</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>F10</f>
+        <f t="shared" si="1"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="H9" s="8" t="str">
@@ -918,11 +920,11 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="G10" s="8" t="str">
-        <f>F11</f>
+        <f t="shared" si="1"/>
         <v>Garner, Jennifer</v>
       </c>
       <c r="H10" s="8"/>

</xml_diff>

<commit_message>
Approval of Olu's problem statement
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134D2698-CE40-9047-A689-7380B407DF7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473FBE45-0FA6-3D4B-BE32-F7B30B4BF872}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13120" yWindow="1420" windowWidth="29220" windowHeight="23140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$11</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,7 +705,7 @@
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="str">
-        <f>A4</f>
+        <f t="shared" ref="F3:F10" si="0">A4</f>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="G3" s="8" t="str">
@@ -739,23 +739,23 @@
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>Motamer, Vajiheh</v>
       </c>
       <c r="G4" s="8" t="str">
-        <f>F5</f>
+        <f t="shared" ref="G4:G10" si="1">F5</f>
         <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="H4" s="8" t="str">
-        <f t="shared" ref="G4:J6" si="0">G5</f>
+        <f t="shared" ref="H4:J6" si="2">G5</f>
         <v>Sekis, Karol</v>
       </c>
       <c r="I4" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="J4" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>White, Robert</v>
       </c>
       <c r="K4" s="10"/>
@@ -771,23 +771,23 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="G5" s="8" t="str">
-        <f>F6</f>
+        <f t="shared" si="1"/>
         <v>Sekis, Karol</v>
       </c>
       <c r="H5" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="I5" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>White, Robert</v>
       </c>
       <c r="J5" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="K5" s="10"/>
@@ -800,26 +800,28 @@
         <v>23</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>Sekis, Karol</v>
       </c>
       <c r="G6" s="8" t="str">
-        <f>F7</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="H6" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>White, Robert</v>
       </c>
       <c r="I6" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="J6" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="K6" s="10"/>
@@ -833,11 +835,11 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">Srinivasan, Malavika </v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>F8</f>
+        <f t="shared" si="1"/>
         <v>White, Robert</v>
       </c>
       <c r="H7" s="8" t="str">
@@ -865,11 +867,11 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>White, Robert</v>
       </c>
       <c r="G8" s="8" t="str">
-        <f>F9</f>
+        <f t="shared" si="1"/>
         <v>Wu, Qirui</v>
       </c>
       <c r="H8" s="8"/>
@@ -888,11 +890,11 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>Wu, Qirui</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>F10</f>
+        <f t="shared" si="1"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="H9" s="8" t="str">
@@ -918,11 +920,11 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="G10" s="8" t="str">
-        <f>F11</f>
+        <f t="shared" si="1"/>
         <v>Garner, Jennifer</v>
       </c>
       <c r="H10" s="8"/>

</xml_diff>

<commit_message>
Updates to repos - correct class list, assign reviewers for written docs
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D935DD-8C37-A643-8B5A-83B4AD11D06C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749CC724-1E69-F945-BD81-1524DE317FD4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -111,10 +111,10 @@
     <t xml:space="preserve">Srinivasan, Malavika </t>
   </si>
   <si>
-    <t>Wu, Qirui</t>
-  </si>
-  <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>https://github.com/karolserkis/CAS-741-Pendula</t>
   </si>
 </sst>
 </file>
@@ -625,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,11 +701,11 @@
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="str">
-        <f t="shared" ref="F3:F10" si="0">A4</f>
+        <f t="shared" ref="F3:G9" si="0">A4</f>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="G3" s="8" t="str">
@@ -735,7 +735,7 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="str">
@@ -743,11 +743,11 @@
         <v>Motamer, Vajiheh</v>
       </c>
       <c r="G4" s="8" t="str">
-        <f t="shared" ref="G4:G10" si="1">F5</f>
+        <f t="shared" ref="G4:G9" si="1">F5</f>
         <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="H4" s="8" t="str">
-        <f t="shared" ref="H4:J6" si="2">G5</f>
+        <f t="shared" ref="H4:J9" si="2">G5</f>
         <v>Sekis, Karol</v>
       </c>
       <c r="I4" s="8" t="str">
@@ -801,7 +801,7 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="str">
@@ -822,7 +822,7 @@
       </c>
       <c r="J6" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>MacLachlan, Brooks</v>
+        <v>Garner, Jennifer</v>
       </c>
       <c r="K6" s="10"/>
     </row>
@@ -830,7 +830,9 @@
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -843,16 +845,16 @@
         <v>White, Robert</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f>G9</f>
+        <f t="shared" si="2"/>
         <v>Zlitni, Hanane</v>
       </c>
       <c r="I7" s="8" t="str">
-        <f>H9</f>
+        <f t="shared" si="2"/>
+        <v>Garner, Jennifer</v>
+      </c>
+      <c r="J7" s="8" t="str">
+        <f t="shared" si="2"/>
         <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="J7" s="8" t="e">
-        <f>I9</f>
-        <v>#REF!</v>
       </c>
       <c r="K7" s="10"/>
     </row>
@@ -872,11 +874,20 @@
       </c>
       <c r="G8" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>Wu, Qirui</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+        <v>Zlitni, Hanane</v>
+      </c>
+      <c r="H8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Garner, Jennifer</v>
+      </c>
+      <c r="I8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>MacLachlan, Brooks</v>
+      </c>
+      <c r="J8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Motamer, Vajiheh</v>
+      </c>
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -888,91 +899,70 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Wu, Qirui</v>
+        <v>Zlitni, Hanane</v>
       </c>
       <c r="G9" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>Zlitni, Hanane</v>
+        <v>Garner, Jennifer</v>
       </c>
       <c r="H9" s="8" t="str">
-        <f>G11</f>
+        <f t="shared" si="2"/>
         <v>MacLachlan, Brooks</v>
       </c>
-      <c r="I9" s="8" t="e">
-        <f>H11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J9" s="8" t="e">
-        <f>I11</f>
-        <v>#REF!</v>
+      <c r="I9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Motamer, Vajiheh</v>
+      </c>
+      <c r="J9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Owojaiye, Oluwaseun</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Zlitni, Hanane</v>
-      </c>
-      <c r="G10" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="str">
         <f>A3</f>
         <v>Garner, Jennifer</v>
       </c>
-      <c r="G11" s="8" t="str">
+      <c r="G10" s="8" t="str">
         <f>F3</f>
         <v>MacLachlan, Brooks</v>
       </c>
-      <c r="H11" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I11" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K11" s="10"/>
+      <c r="H10" s="8" t="str">
+        <f>G3</f>
+        <v>Motamer, Vajiheh</v>
+      </c>
+      <c r="I10" s="8" t="str">
+        <f>H3</f>
+        <v>Owojaiye, Oluwaseun</v>
+      </c>
+      <c r="J10" s="8" t="str">
+        <f>I3</f>
+        <v>Sekis, Karol</v>
+      </c>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Approval of Vajiheh problem statement
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749CC724-1E69-F945-BD81-1524DE317FD4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E414228-CF3F-CF40-83C4-D329D90C6E4D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3180" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -628,7 +628,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,7 +705,7 @@
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="str">
-        <f t="shared" ref="F3:G9" si="0">A4</f>
+        <f t="shared" ref="F3:F9" si="0">A4</f>
         <v>MacLachlan, Brooks</v>
       </c>
       <c r="G3" s="8" t="str">
@@ -768,7 +768,9 @@
         <v>22</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Approval of Malavika's problem statement
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E414228-CF3F-CF40-83C4-D329D90C6E4D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB3401D-C8B7-7942-A1B5-EB97B80A6259}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="3180" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -628,7 +628,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -868,7 +868,9 @@
         <v>20</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Hyperlink added to Repos.xlsx
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB3401D-C8B7-7942-A1B5-EB97B80A6259}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55598336-0405-F84D-9A7B-E755D9F303F6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3180" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -628,7 +628,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,7 +832,7 @@
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="8"/>
@@ -972,6 +972,7 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{8860323E-E796-6542-9DBE-B172243EFBE2}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{05EFC813-9F41-BE47-A926-BACE82D050AB}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update to show all projects have been approved
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55598336-0405-F84D-9A7B-E755D9F303F6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D5845-31B4-6B45-998F-A2AFC620CD7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="43300" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,7 +836,9 @@
         <v>27</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Some initial work preparing the course for the coming term, still more to do ...
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683D5845-31B4-6B45-998F-A2AFC620CD7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF92534-EDF2-4543-A2BD-42789FBE1EAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="43300" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$B$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$10</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -51,9 +51,6 @@
     <t>SRS</t>
   </si>
   <si>
-    <t>REVIEWED BY THE PERSON LISTED BELOW</t>
-  </si>
-  <si>
     <t>VnV Plan</t>
   </si>
   <si>
@@ -66,55 +63,58 @@
     <t>Implement</t>
   </si>
   <si>
-    <t>Garner, Jennifer</t>
-  </si>
-  <si>
-    <t>MacLachlan, Brooks</t>
-  </si>
-  <si>
-    <t>Motamer, Vajiheh</t>
-  </si>
-  <si>
-    <t>Owojaiye, Oluwaseun</t>
-  </si>
-  <si>
-    <t>White, Robert</t>
-  </si>
-  <si>
-    <t>Zlitni, Hanane</t>
-  </si>
-  <si>
-    <t>https://github.com/hananezlitni/HZ-CAS741-Project</t>
-  </si>
-  <si>
-    <t>https://github.com/PeaWagon/Kaplan</t>
-  </si>
-  <si>
-    <t>https://github.com/whitere123/CAS741_REW</t>
-  </si>
-  <si>
-    <t>https://github.com/Malavika-Srinivasan/CAS741</t>
-  </si>
-  <si>
-    <t>https://github.com/smiths/caseStudies/tree/master/CaseStudies/ssp</t>
-  </si>
-  <si>
-    <t>https://github.com/smiths/caseStudies/tree/master/CaseStudies/glass</t>
-  </si>
-  <si>
-    <t>https://github.com/smiths/caseStudies/tree/master/CaseStudies/gamephys</t>
-  </si>
-  <si>
-    <t>Sekis, Karol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srinivasan, Malavika </t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>https://github.com/karolserkis/CAS-741-Pendula</t>
+    <t>Stdnt 1</t>
+  </si>
+  <si>
+    <t>Repo url</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Project name</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Second Reviewer - Reviewed BY the person listed below</t>
+  </si>
+  <si>
+    <t>Stdnt 2</t>
+  </si>
+  <si>
+    <t>Stdnt 3</t>
+  </si>
+  <si>
+    <t>Stdnt 4</t>
+  </si>
+  <si>
+    <t>Stdnt 5</t>
+  </si>
+  <si>
+    <t>Stdnt 6</t>
+  </si>
+  <si>
+    <t>Stdnt 7</t>
+  </si>
+  <si>
+    <t>Stdnt 8</t>
+  </si>
+  <si>
+    <t>In the cases where a presentation is made, the expert reviewer and the second reviewer will be assigned to ask questions during/after the presentation</t>
+  </si>
+  <si>
+    <t>Domain expert will also be assigned document inspection tasks by the document author</t>
+  </si>
+  <si>
+    <t>Domain expert will also implement one module</t>
   </si>
 </sst>
 </file>
@@ -305,7 +305,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -322,6 +322,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="23" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -625,357 +630,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.83203125" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" customWidth="1"/>
-    <col min="9" max="9" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="62.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" customWidth="1"/>
+    <col min="11" max="11" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="str">
-        <f t="shared" ref="F3:F9" si="0">A4</f>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="G3" s="8" t="str">
-        <f>F4</f>
-        <v>Motamer, Vajiheh</v>
-      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="8" t="str">
-        <f>G4</f>
-        <v>Owojaiye, Oluwaseun</v>
+        <f t="shared" ref="H3:H9" si="0">A4</f>
+        <v>Stdnt 2</v>
       </c>
       <c r="I3" s="8" t="str">
         <f>H4</f>
-        <v>Sekis, Karol</v>
+        <v>Stdnt 3</v>
       </c>
       <c r="J3" s="8" t="str">
         <f>I4</f>
-        <v xml:space="preserve">Srinivasan, Malavika </v>
-      </c>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>Stdnt 4</v>
+      </c>
+      <c r="K3" s="8" t="str">
+        <f>J4</f>
+        <v>Stdnt 5</v>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f>K4</f>
+        <v>Stdnt 6</v>
+      </c>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Stdnt 3</v>
+      </c>
+      <c r="I4" s="8" t="str">
+        <f t="shared" ref="I4:I9" si="1">H5</f>
+        <v>Stdnt 4</v>
+      </c>
+      <c r="J4" s="8" t="str">
+        <f t="shared" ref="J4:L9" si="2">I5</f>
+        <v>Stdnt 5</v>
+      </c>
+      <c r="K4" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 6</v>
+      </c>
+      <c r="L4" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 7</v>
+      </c>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Stdnt 4</v>
+      </c>
+      <c r="I5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Stdnt 5</v>
+      </c>
+      <c r="J5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 6</v>
+      </c>
+      <c r="K5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 7</v>
+      </c>
+      <c r="L5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 8</v>
+      </c>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Stdnt 5</v>
+      </c>
+      <c r="I6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Stdnt 6</v>
+      </c>
+      <c r="J6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 7</v>
+      </c>
+      <c r="K6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 8</v>
+      </c>
+      <c r="L6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 1</v>
+      </c>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="str">
+      <c r="B7" s="7"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Motamer, Vajiheh</v>
-      </c>
-      <c r="G4" s="8" t="str">
-        <f t="shared" ref="G4:G9" si="1">F5</f>
-        <v>Owojaiye, Oluwaseun</v>
-      </c>
-      <c r="H4" s="8" t="str">
-        <f t="shared" ref="H4:J9" si="2">G5</f>
-        <v>Sekis, Karol</v>
-      </c>
-      <c r="I4" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">Srinivasan, Malavika </v>
-      </c>
-      <c r="J4" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>White, Robert</v>
-      </c>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="8" t="s">
+        <v>Stdnt 6</v>
+      </c>
+      <c r="I7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Stdnt 7</v>
+      </c>
+      <c r="J7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 8</v>
+      </c>
+      <c r="K7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 1</v>
+      </c>
+      <c r="L7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 2</v>
+      </c>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="str">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Owojaiye, Oluwaseun</v>
-      </c>
-      <c r="G5" s="8" t="str">
+        <v>Stdnt 7</v>
+      </c>
+      <c r="I8" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>Sekis, Karol</v>
-      </c>
-      <c r="H5" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">Srinivasan, Malavika </v>
-      </c>
-      <c r="I5" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>White, Robert</v>
-      </c>
-      <c r="J5" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Zlitni, Hanane</v>
-      </c>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+        <v>Stdnt 8</v>
+      </c>
+      <c r="J8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 1</v>
+      </c>
+      <c r="K8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 2</v>
+      </c>
+      <c r="L8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 3</v>
+      </c>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="str">
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Sekis, Karol</v>
-      </c>
-      <c r="G6" s="8" t="str">
+        <v>Stdnt 8</v>
+      </c>
+      <c r="I9" s="8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">Srinivasan, Malavika </v>
-      </c>
-      <c r="H6" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>White, Robert</v>
-      </c>
-      <c r="I6" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Zlitni, Hanane</v>
-      </c>
-      <c r="J6" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+        <v>Stdnt 1</v>
+      </c>
+      <c r="J9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 2</v>
+      </c>
+      <c r="K9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 3</v>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Stdnt 4</v>
+      </c>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Srinivasan, Malavika </v>
-      </c>
-      <c r="G7" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>White, Robert</v>
-      </c>
-      <c r="H7" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Zlitni, Hanane</v>
-      </c>
-      <c r="I7" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="J7" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>White, Robert</v>
-      </c>
-      <c r="G8" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Zlitni, Hanane</v>
-      </c>
-      <c r="H8" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="I8" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="J8" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Motamer, Vajiheh</v>
-      </c>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Zlitni, Hanane</v>
-      </c>
-      <c r="G9" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="H9" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="I9" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Motamer, Vajiheh</v>
-      </c>
-      <c r="J9" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Owojaiye, Oluwaseun</v>
-      </c>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="B10" s="7"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="str">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="str">
         <f>A3</f>
-        <v>Garner, Jennifer</v>
-      </c>
-      <c r="G10" s="8" t="str">
-        <f>F3</f>
-        <v>MacLachlan, Brooks</v>
-      </c>
-      <c r="H10" s="8" t="str">
-        <f>G3</f>
-        <v>Motamer, Vajiheh</v>
+        <v>Stdnt 1</v>
       </c>
       <c r="I10" s="8" t="str">
         <f>H3</f>
-        <v>Owojaiye, Oluwaseun</v>
+        <v>Stdnt 2</v>
       </c>
       <c r="J10" s="8" t="str">
         <f>I3</f>
-        <v>Sekis, Karol</v>
-      </c>
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>Stdnt 3</v>
+      </c>
+      <c r="K10" s="8" t="str">
+        <f>J3</f>
+        <v>Stdnt 4</v>
+      </c>
+      <c r="L10" s="8" t="str">
+        <f>K3</f>
+        <v>Stdnt 5</v>
+      </c>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{8860323E-E796-6542-9DBE-B172243EFBE2}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{05EFC813-9F41-BE47-A926-BACE82D050AB}"/>
-  </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to list of student repositories
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,33 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73581214-96A1-4F4A-A46D-F0A0BFCFD414}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1FCC18-046C-E841-B9E6-1FCCC1037DCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="3420" windowWidth="43300" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="2480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$E$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$E$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -60,18 +54,6 @@
     <t>VnV Plan</t>
   </si>
   <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>MIS</t>
-  </si>
-  <si>
-    <t>Implement</t>
-  </si>
-  <si>
-    <t>Repo url</t>
-  </si>
-  <si>
     <t>Project Name</t>
   </si>
   <si>
@@ -105,27 +87,15 @@
     <t>Bo Cao</t>
   </si>
   <si>
-    <t>Ge Chen</t>
-  </si>
-  <si>
-    <t>Mohammad Ali Daeian</t>
-  </si>
-  <si>
     <t>Ao Dong</t>
   </si>
   <si>
     <t>Peter Michalski</t>
   </si>
   <si>
-    <t>Lekhani Ray</t>
-  </si>
-  <si>
     <t>Sasha Soraine</t>
   </si>
   <si>
-    <t>Weiyi Wu</t>
-  </si>
-  <si>
     <t>Zhi Zhang</t>
   </si>
   <si>
@@ -144,25 +114,43 @@
     <t>cheng54@mcmaster.ca</t>
   </si>
   <si>
-    <t>daeianm@mcmaster.ca</t>
-  </si>
-  <si>
     <t>donga9@mcmaster.ca</t>
   </si>
   <si>
     <t>michap@mcmaster.ca</t>
   </si>
   <si>
-    <t>rayl1@mcmaster.ca</t>
-  </si>
-  <si>
     <t>sorainsm@mcmaster.ca</t>
   </si>
   <si>
-    <t>wuw62@mcmaster.ca</t>
-  </si>
-  <si>
     <t>zhangz1@mcmaster.ca</t>
+  </si>
+  <si>
+    <t>https://github.com/deemaalomair1/CAS741_project</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>https://github.com/Ao99/CAS741</t>
+  </si>
+  <si>
+    <t>https://github.com/peter-michalski/CAS741project</t>
+  </si>
+  <si>
+    <t>https://github.com/best-zhang-zhi/CAS741Project</t>
+  </si>
+  <si>
+    <t>Ge Chen (Colin)</t>
+  </si>
+  <si>
+    <t>Sharon Oh</t>
+  </si>
+  <si>
+    <t>wuy@mcmaster.ca</t>
+  </si>
+  <si>
+    <t>MG + MIS</t>
   </si>
 </sst>
 </file>
@@ -215,9 +203,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,7 +323,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -363,10 +350,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="23" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="23" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="23"/>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -670,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,22 +678,20 @@
     <col min="10" max="10" width="17.33203125" customWidth="1"/>
     <col min="11" max="11" width="18.5" customWidth="1"/>
     <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
@@ -718,20 +704,18 @@
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
-      <c r="N1" s="14"/>
+      <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
@@ -743,7 +727,7 @@
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>5</v>
@@ -752,456 +736,360 @@
         <v>6</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>9</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
       <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17" t="str">
-        <f t="shared" ref="J3:J9" si="0">B4</f>
+      <c r="G3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16" t="str">
+        <f t="shared" ref="J3:J7" si="0">B4</f>
         <v>Bo Cao</v>
       </c>
-      <c r="K3" s="17" t="str">
+      <c r="K3" s="16" t="str">
         <f>J4</f>
-        <v>Ge Chen</v>
-      </c>
-      <c r="L3" s="17" t="str">
+        <v>Ge Chen (Colin)</v>
+      </c>
+      <c r="L3" s="16" t="str">
         <f>K4</f>
-        <v>Mohammad Ali Daeian</v>
-      </c>
-      <c r="M3" s="17" t="str">
-        <f>L4</f>
         <v>Ao Dong</v>
       </c>
-      <c r="N3" s="17" t="str">
-        <f>M4</f>
-        <v>Peter Michalski</v>
-      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
       <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-    </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="str">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Ge Chen</v>
-      </c>
-      <c r="K4" s="17" t="str">
-        <f t="shared" ref="K4:K9" si="1">J5</f>
-        <v>Mohammad Ali Daeian</v>
-      </c>
-      <c r="L4" s="17" t="str">
-        <f t="shared" ref="L4:N9" si="2">K5</f>
+        <v>Ge Chen (Colin)</v>
+      </c>
+      <c r="K4" s="16" t="str">
+        <f t="shared" ref="K4:K7" si="1">J5</f>
         <v>Ao Dong</v>
       </c>
-      <c r="M4" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="L4" s="16" t="str">
+        <f t="shared" ref="L4:L7" si="2">K5</f>
         <v>Peter Michalski</v>
       </c>
-      <c r="N4" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Lekhani Ray</v>
-      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
       <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-    </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:18" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
-        <f t="shared" ref="A5:A12" si="3">A4+1</f>
+        <f t="shared" ref="A5:A10" si="3">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17" t="str">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Mohammad Ali Daeian</v>
-      </c>
-      <c r="K5" s="17" t="str">
+        <v>Ao Dong</v>
+      </c>
+      <c r="K5" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Ao Dong</v>
-      </c>
-      <c r="L5" s="17" t="str">
-        <f t="shared" si="2"/>
         <v>Peter Michalski</v>
       </c>
-      <c r="M5" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Lekhani Ray</v>
-      </c>
-      <c r="N5" s="17" t="str">
+      <c r="L5" s="16" t="str">
         <f t="shared" si="2"/>
         <v>Sasha Soraine</v>
       </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
       <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-    </row>
-    <row r="6" spans="1:17" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17" t="str">
+      <c r="E6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Ao Dong</v>
-      </c>
-      <c r="K6" s="17" t="str">
+        <v>Peter Michalski</v>
+      </c>
+      <c r="K6" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Peter Michalski</v>
-      </c>
-      <c r="L6" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Lekhani Ray</v>
-      </c>
-      <c r="M6" s="17" t="str">
-        <f t="shared" si="2"/>
         <v>Sasha Soraine</v>
       </c>
-      <c r="N6" s="17" t="str">
+      <c r="L6" s="16" t="str">
         <f t="shared" si="2"/>
         <v>Deema Alomair</v>
       </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
       <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-    </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17" t="str">
+      <c r="E7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Peter Michalski</v>
-      </c>
-      <c r="K7" s="17" t="str">
+        <v>Sasha Soraine</v>
+      </c>
+      <c r="K7" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Lekhani Ray</v>
-      </c>
-      <c r="L7" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Sasha Soraine</v>
-      </c>
-      <c r="M7" s="17" t="str">
-        <f t="shared" si="2"/>
         <v>Deema Alomair</v>
       </c>
-      <c r="N7" s="17" t="str">
+      <c r="L7" s="16" t="str">
         <f t="shared" si="2"/>
         <v>Bo Cao</v>
       </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-    </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>Lekhani Ray</v>
-      </c>
-      <c r="K8" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Sasha Soraine</v>
-      </c>
-      <c r="L8" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16" t="str">
+        <f>B3</f>
         <v>Deema Alomair</v>
       </c>
-      <c r="M8" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="K8" s="16" t="str">
+        <f t="shared" ref="K8:L10" si="4">J3</f>
         <v>Bo Cao</v>
       </c>
-      <c r="N8" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Ge Chen</v>
-      </c>
+      <c r="L8" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>Ge Chen (Colin)</v>
+      </c>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-    </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>Sasha Soraine</v>
-      </c>
-      <c r="K9" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>Deema Alomair</v>
-      </c>
-      <c r="L9" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="F9" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16" t="str">
+        <f>B4</f>
         <v>Bo Cao</v>
       </c>
-      <c r="M9" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Ge Chen</v>
-      </c>
-      <c r="N9" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>Mohammad Ali Daeian</v>
-      </c>
+      <c r="K9" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>Ge Chen (Colin)</v>
+      </c>
+      <c r="L9" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>Ao Dong</v>
+      </c>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
       <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-    </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>39</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17" t="str">
-        <f>B3</f>
-        <v>Deema Alomair</v>
-      </c>
-      <c r="K10" s="17" t="str">
-        <f t="shared" ref="K10:N12" si="4">J3</f>
-        <v>Bo Cao</v>
-      </c>
-      <c r="L10" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Ge Chen</v>
-      </c>
-      <c r="M10" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Mohammad Ali Daeian</v>
-      </c>
-      <c r="N10" s="17" t="str">
+      <c r="E10" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16" t="str">
+        <f>B5</f>
+        <v>Ge Chen (Colin)</v>
+      </c>
+      <c r="K10" s="16" t="str">
         <f t="shared" si="4"/>
         <v>Ao Dong</v>
       </c>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-    </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17" t="str">
-        <f>B4</f>
-        <v>Bo Cao</v>
-      </c>
-      <c r="K11" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Ge Chen</v>
-      </c>
-      <c r="L11" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Mohammad Ali Daeian</v>
-      </c>
-      <c r="M11" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Ao Dong</v>
-      </c>
-      <c r="N11" s="17" t="str">
+      <c r="L10" s="16" t="str">
         <f t="shared" si="4"/>
         <v>Peter Michalski</v>
       </c>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
       <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-    </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17" t="s">
+    </row>
+    <row r="12" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17" t="str">
-        <f>B5</f>
-        <v>Ge Chen</v>
-      </c>
-      <c r="K12" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Mohammad Ali Daeian</v>
-      </c>
-      <c r="L12" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Ao Dong</v>
-      </c>
-      <c r="M12" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Peter Michalski</v>
-      </c>
-      <c r="N12" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v>Lekhani Ray</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
       <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-    </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1210,19 +1098,17 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
       <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-    </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1231,18 +1117,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
       <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-    </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1254,54 +1136,52 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-    </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-    </row>
-    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+    </row>
+    <row r="16" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+    </row>
+    <row r="17" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
       <c r="R17"/>
-      <c r="S17"/>
-      <c r="T17"/>
-    </row>
-    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1320,52 +1200,6 @@
       <c r="P18"/>
       <c r="Q18"/>
       <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
-    </row>
-    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
-    </row>
-    <row r="20" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
-      <c r="R20"/>
-      <c r="S20"/>
-      <c r="T20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1373,13 +1207,15 @@
     <hyperlink ref="C3" r:id="rId1" xr:uid="{EF275338-8768-704D-9514-53651BC63C3E}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{C5C3D4B5-50E6-9044-91CC-55C0D86C8F39}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{5E93B0E7-10BB-964A-95A9-9A15457ACF05}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{A9E0065E-70E2-714D-8B65-FA2F3A8094E5}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{99A63936-4E29-9B41-B446-60C325D481D2}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{FDCEAA7B-09B9-394F-9272-06A2E42534F2}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{DC667284-2273-B14B-AB50-ABE2DE99997C}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{C907EC9B-B30E-6F49-99C6-F56985FD93FE}"/>
-    <hyperlink ref="C11" r:id="rId9" xr:uid="{99A18F7E-5960-544E-A1AF-931B9CE95D24}"/>
-    <hyperlink ref="C12" r:id="rId10" xr:uid="{7253496C-EABA-2645-B050-975DBA0B0108}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{99A63936-4E29-9B41-B446-60C325D481D2}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{FDCEAA7B-09B9-394F-9272-06A2E42534F2}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{C907EC9B-B30E-6F49-99C6-F56985FD93FE}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{7253496C-EABA-2645-B050-975DBA0B0108}"/>
+    <hyperlink ref="E3" r:id="rId8" xr:uid="{82DB3A68-C170-F34D-92F3-2B6FA7908C23}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{9DD92EA4-84F2-1740-8AC0-FA06C087B9A1}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{953AEC1E-EA56-644B-A121-BE2F1549DE0D}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{05C67F68-0321-854D-B729-8137B386E25B}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated repo link for Sasha's project
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1FCC18-046C-E841-B9E6-1FCCC1037DCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B243A89-6791-3C44-A7B4-027159CEA664}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="2480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="4480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>MG + MIS</t>
+  </si>
+  <si>
+    <t>https://github.com/sorainsm/library-of-lighting-models</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,7 +949,9 @@
         <v>29</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="16"/>
+      <c r="E8" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="F8" s="19" t="s">
         <v>32</v>
       </c>
@@ -1216,6 +1221,7 @@
     <hyperlink ref="E7" r:id="rId10" xr:uid="{953AEC1E-EA56-644B-A121-BE2F1549DE0D}"/>
     <hyperlink ref="E10" r:id="rId11" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
     <hyperlink ref="C9" r:id="rId12" xr:uid="{05C67F68-0321-854D-B729-8137B386E25B}"/>
+    <hyperlink ref="E8" r:id="rId13" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Addition of url for Bo Cao's repo
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B243A89-6791-3C44-A7B4-027159CEA664}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D8A40D-963F-CF48-8A68-1D6702EED7DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="4480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="4480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>https://github.com/sorainsm/library-of-lighting-models</t>
+  </si>
+  <si>
+    <t>https://github.com/caobo1994/FourierSeries</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,7 +800,9 @@
         <v>25</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="16"/>
+      <c r="E4" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="F4" s="16" t="s">
         <v>32</v>
       </c>
@@ -1222,6 +1227,7 @@
     <hyperlink ref="E10" r:id="rId11" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
     <hyperlink ref="C9" r:id="rId12" xr:uid="{05C67F68-0321-854D-B729-8137B386E25B}"/>
     <hyperlink ref="E8" r:id="rId13" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
+    <hyperlink ref="E4" r:id="rId14" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updates to list of repos for projects
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D8A40D-963F-CF48-8A68-1D6702EED7DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C467EEF-3A6B-6243-A49E-3C611BA9105C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>Project name</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -157,6 +154,24 @@
   </si>
   <si>
     <t>https://github.com/caobo1994/FourierSeries</t>
+  </si>
+  <si>
+    <t>Mass-Mass Stoichiometry Problem</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Fourier Series</t>
+  </si>
+  <si>
+    <t>Medical Imaging Applications</t>
+  </si>
+  <si>
+    <t>Lattice Boltzmann Solvers</t>
+  </si>
+  <si>
+    <t>Light</t>
   </si>
 </sst>
 </file>
@@ -667,7 +682,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,13 +703,13 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>7</v>
@@ -710,10 +725,10 @@
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="13"/>
@@ -733,7 +748,7 @@
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>5</v>
@@ -742,33 +757,33 @@
         <v>6</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="E3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>32</v>
-      </c>
       <c r="G3" s="16" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -794,20 +809,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="E4" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -833,18 +850,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -864,26 +881,28 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="E6" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -909,20 +928,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E7" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -948,20 +969,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="E8" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
@@ -987,18 +1010,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>38</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="16"/>
       <c r="F9" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
@@ -1024,20 +1047,20 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
@@ -1077,7 +1100,7 @@
     <row r="12" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="13"/>
@@ -1096,7 +1119,7 @@
     <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
@@ -1115,7 +1138,7 @@
     <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>

</xml_diff>

<commit_message>
Updates to list of approved problem statements
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C467EEF-3A6B-6243-A49E-3C611BA9105C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A53DD3-3ABC-634A-B341-4C43AB080C42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,16 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$E$8</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -162,9 +168,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Fourier Series</t>
-  </si>
-  <si>
     <t>Medical Imaging Applications</t>
   </si>
   <si>
@@ -172,6 +175,9 @@
   </si>
   <si>
     <t>Light</t>
+  </si>
+  <si>
+    <t>Fourier Series Library</t>
   </si>
 </sst>
 </file>
@@ -682,7 +688,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,7 +821,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>40</v>
@@ -824,7 +830,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -893,7 +899,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>32</v>
@@ -934,7 +940,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>33</v>
@@ -943,7 +949,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -975,7 +981,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
All students now have repo urls
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A53DD3-3ABC-634A-B341-4C43AB080C42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B8478E-CA09-D54B-835C-7D3ED9F41DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="4480" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4480" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -147,12 +147,6 @@
     <t>Ge Chen (Colin)</t>
   </si>
   <si>
-    <t>Sharon Oh</t>
-  </si>
-  <si>
-    <t>wuy@mcmaster.ca</t>
-  </si>
-  <si>
     <t>MG + MIS</t>
   </si>
   <si>
@@ -178,6 +172,27 @@
   </si>
   <si>
     <t>Fourier Series Library</t>
+  </si>
+  <si>
+    <t>https://github.com/bigship/CAS741</t>
+  </si>
+  <si>
+    <t>Machine Learning App</t>
+  </si>
+  <si>
+    <t>Sharon Wu</t>
+  </si>
+  <si>
+    <t>sharyuwu@gmail.com</t>
+  </si>
+  <si>
+    <t>https://github.com/sharyuwu/optimum-tilt-of-solar-panels</t>
+  </si>
+  <si>
+    <t>Solar Panel Tilt</t>
+  </si>
+  <si>
+    <t>Polynomial Interpolation</t>
   </si>
 </sst>
 </file>
@@ -688,7 +703,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,7 +778,7 @@
         <v>6</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
@@ -780,7 +795,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>30</v>
@@ -789,7 +804,7 @@
         <v>31</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -821,16 +836,16 @@
         <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -861,8 +876,12 @@
       <c r="C5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="16"/>
+      <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="F5" s="16" t="s">
         <v>31</v>
       </c>
@@ -899,7 +918,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>32</v>
@@ -940,7 +959,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>33</v>
@@ -949,7 +968,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -981,10 +1000,10 @@
         <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>31</v>
@@ -1016,13 +1035,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="F9" s="19" t="s">
         <v>31</v>
       </c>
@@ -1058,7 +1081,9 @@
       <c r="C10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="E10" s="20" t="s">
         <v>34</v>
       </c>
@@ -1254,9 +1279,10 @@
     <hyperlink ref="E6" r:id="rId9" xr:uid="{9DD92EA4-84F2-1740-8AC0-FA06C087B9A1}"/>
     <hyperlink ref="E7" r:id="rId10" xr:uid="{953AEC1E-EA56-644B-A121-BE2F1549DE0D}"/>
     <hyperlink ref="E10" r:id="rId11" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
-    <hyperlink ref="C9" r:id="rId12" xr:uid="{05C67F68-0321-854D-B729-8137B386E25B}"/>
-    <hyperlink ref="E8" r:id="rId13" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
-    <hyperlink ref="E4" r:id="rId14" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
+    <hyperlink ref="E8" r:id="rId12" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
+    <hyperlink ref="E4" r:id="rId13" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
+    <hyperlink ref="E5" r:id="rId14" xr:uid="{BD77D372-E5FE-7348-A005-C40823ABB1DE}"/>
+    <hyperlink ref="E9" r:id="rId15" xr:uid="{7F6B845B-29C9-EE47-9761-BEFBD243476C}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Approval of Colin Chen's project
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B8478E-CA09-D54B-835C-7D3ED9F41DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C367AC-BF87-D247-B1E4-C6871AB88365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>https://github.com/bigship/CAS741</t>
   </si>
   <si>
-    <t>Machine Learning App</t>
-  </si>
-  <si>
     <t>Sharon Wu</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>Polynomial Interpolation</t>
+  </si>
+  <si>
+    <t>HealthyFood</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,7 +877,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>45</v>
@@ -886,7 +886,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -1035,16 +1035,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>48</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>31</v>
@@ -1082,7 +1082,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added permission for Sasha's project to Repo.xlsx
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C367AC-BF87-D247-B1E4-C6871AB88365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8587312D-74E4-EE48-A7B7-610AE8B39FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -703,7 +703,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1009,7 @@
         <v>31</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>

</xml_diff>

<commit_message>
Updates to project approvals
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8587312D-74E4-EE48-A7B7-610AE8B39FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC281015-AADB-594C-AD9C-244064E90352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,16 +18,10 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$E$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -168,9 +162,6 @@
     <t>Lattice Boltzmann Solvers</t>
   </si>
   <si>
-    <t>Light</t>
-  </si>
-  <si>
     <t>Fourier Series Library</t>
   </si>
   <si>
@@ -186,13 +177,16 @@
     <t>https://github.com/sharyuwu/optimum-tilt-of-solar-panels</t>
   </si>
   <si>
-    <t>Solar Panel Tilt</t>
-  </si>
-  <si>
-    <t>Polynomial Interpolation</t>
-  </si>
-  <si>
     <t>HealthyFood</t>
+  </si>
+  <si>
+    <t>Double pendulum</t>
+  </si>
+  <si>
+    <t>Library of Lighting Models</t>
+  </si>
+  <si>
+    <t>Optimal Solar Panel Tilt</t>
   </si>
 </sst>
 </file>
@@ -703,7 +697,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,7 +830,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>38</v>
@@ -877,10 +871,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>31</v>
@@ -1000,7 +994,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>37</v>
@@ -1035,22 +1029,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>47</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>48</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
@@ -1082,7 +1076,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>34</v>
@@ -1091,7 +1085,7 @@
         <v>31</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>

</xml_diff>

<commit_message>
Correction of second reviewers in list or repositories
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC281015-AADB-594C-AD9C-244064E90352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF876D20-D6D5-544C-AD5C-9D86144F27A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     <t>Sharon Wu</t>
   </si>
   <si>
-    <t>sharyuwu@gmail.com</t>
-  </si>
-  <si>
     <t>https://github.com/sharyuwu/optimum-tilt-of-solar-panels</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Optimal Solar Panel Tilt</t>
+  </si>
+  <si>
+    <t>wuy324@mcmaster.ca</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,7 +803,7 @@
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16" t="str">
-        <f t="shared" ref="J3:J7" si="0">B4</f>
+        <f t="shared" ref="J3:J10" si="0">B4</f>
         <v>Bo Cao</v>
       </c>
       <c r="K3" s="16" t="str">
@@ -848,11 +848,11 @@
         <v>Ge Chen (Colin)</v>
       </c>
       <c r="K4" s="16" t="str">
-        <f t="shared" ref="K4:K7" si="1">J5</f>
+        <f>J5</f>
         <v>Ao Dong</v>
       </c>
       <c r="L4" s="16" t="str">
-        <f t="shared" ref="L4:L7" si="2">K5</f>
+        <f t="shared" ref="L4:L10" si="1">K5</f>
         <v>Peter Michalski</v>
       </c>
       <c r="M4" s="13"/>
@@ -861,7 +861,7 @@
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
-        <f t="shared" ref="A5:A10" si="3">A4+1</f>
+        <f t="shared" ref="A5:A10" si="2">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -871,7 +871,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>44</v>
@@ -889,11 +889,11 @@
         <v>Ao Dong</v>
       </c>
       <c r="K5" s="16" t="str">
+        <f>J6</f>
+        <v>Peter Michalski</v>
+      </c>
+      <c r="L5" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Peter Michalski</v>
-      </c>
-      <c r="L5" s="16" t="str">
-        <f t="shared" si="2"/>
         <v>Sasha Soraine</v>
       </c>
       <c r="M5" s="13"/>
@@ -902,7 +902,7 @@
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -930,12 +930,12 @@
         <v>Peter Michalski</v>
       </c>
       <c r="K6" s="16" t="str">
+        <f>J7</f>
+        <v>Sasha Soraine</v>
+      </c>
+      <c r="L6" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Sasha Soraine</v>
-      </c>
-      <c r="L6" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v>Deema Alomair</v>
+        <v>Sharon Wu</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -943,7 +943,7 @@
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -971,12 +971,12 @@
         <v>Sasha Soraine</v>
       </c>
       <c r="K7" s="16" t="str">
+        <f>J8</f>
+        <v>Sharon Wu</v>
+      </c>
+      <c r="L7" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Deema Alomair</v>
-      </c>
-      <c r="L7" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v>Bo Cao</v>
+        <v>Zhi Zhang</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -984,7 +984,7 @@
     </row>
     <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -994,7 +994,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>37</v>
@@ -1008,16 +1008,16 @@
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16" t="str">
-        <f>B3</f>
+        <f t="shared" si="0"/>
+        <v>Sharon Wu</v>
+      </c>
+      <c r="K8" s="16" t="str">
+        <f>J9</f>
+        <v>Zhi Zhang</v>
+      </c>
+      <c r="L8" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>Deema Alomair</v>
-      </c>
-      <c r="K8" s="16" t="str">
-        <f t="shared" ref="K8:L10" si="4">J3</f>
-        <v>Bo Cao</v>
-      </c>
-      <c r="L8" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v>Ge Chen (Colin)</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
@@ -1025,20 +1025,20 @@
     </row>
     <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>47</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>31</v>
@@ -1049,16 +1049,16 @@
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16" t="str">
-        <f>B4</f>
+        <f t="shared" si="0"/>
+        <v>Zhi Zhang</v>
+      </c>
+      <c r="K9" s="16" t="str">
+        <f>J10</f>
+        <v>Deema Alomair</v>
+      </c>
+      <c r="L9" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>Bo Cao</v>
-      </c>
-      <c r="K9" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v>Ge Chen (Colin)</v>
-      </c>
-      <c r="L9" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v>Ao Dong</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1076,7 +1076,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>34</v>
@@ -1090,16 +1090,16 @@
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="str">
-        <f>B5</f>
+        <f>B3</f>
+        <v>Deema Alomair</v>
+      </c>
+      <c r="K10" s="16" t="str">
+        <f>J3</f>
+        <v>Bo Cao</v>
+      </c>
+      <c r="L10" s="16" t="str">
+        <f>K3</f>
         <v>Ge Chen (Colin)</v>
-      </c>
-      <c r="K10" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v>Ao Dong</v>
-      </c>
-      <c r="L10" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v>Peter Michalski</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -1277,6 +1277,7 @@
     <hyperlink ref="E4" r:id="rId13" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
     <hyperlink ref="E5" r:id="rId14" xr:uid="{BD77D372-E5FE-7348-A005-C40823ABB1DE}"/>
     <hyperlink ref="E9" r:id="rId15" xr:uid="{7F6B845B-29C9-EE47-9761-BEFBD243476C}"/>
+    <hyperlink ref="C9" r:id="rId16" xr:uid="{DE229207-DE5E-2148-A086-7C91C16E5E4D}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Addition of GitHub Ids
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF876D20-D6D5-544C-AD5C-9D86144F27A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A02154-E211-BC4D-AB59-78669FCE0AAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$E$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$F$8</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -187,6 +187,33 @@
   </si>
   <si>
     <t>wuy324@mcmaster.ca</t>
+  </si>
+  <si>
+    <t>GitHub ID</t>
+  </si>
+  <si>
+    <t>deemaalomair1</t>
+  </si>
+  <si>
+    <t>caobo1994</t>
+  </si>
+  <si>
+    <t>bigship</t>
+  </si>
+  <si>
+    <t>Ao99</t>
+  </si>
+  <si>
+    <t>peter-michalski</t>
+  </si>
+  <si>
+    <t>sorainsm</t>
+  </si>
+  <si>
+    <t>sharyuwu</t>
+  </si>
+  <si>
+    <t>best-zhang-zhi</t>
   </si>
 </sst>
 </file>
@@ -359,7 +386,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -391,6 +418,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="23"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -694,29 +724,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="3" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
@@ -726,99 +756,106 @@
       <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="13"/>
+      <c r="L1" s="12"/>
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
-    </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="P2" s="13"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="16"/>
       <c r="I3" s="16"/>
-      <c r="J3" s="16" t="str">
-        <f t="shared" ref="J3:J10" si="0">B4</f>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="str">
+        <f>B4</f>
         <v>Bo Cao</v>
-      </c>
-      <c r="K3" s="16" t="str">
-        <f>J4</f>
-        <v>Ge Chen (Colin)</v>
       </c>
       <c r="L3" s="16" t="str">
         <f>K4</f>
+        <v>Ge Chen (Colin)</v>
+      </c>
+      <c r="M3" s="16" t="str">
+        <f>L4</f>
         <v>Ao Dong</v>
       </c>
-      <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
-    </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="13"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <f>A3+1</f>
         <v>2</v>
@@ -829,39 +866,42 @@
       <c r="C4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="G4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="H4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="16"/>
       <c r="I4" s="16"/>
-      <c r="J4" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16" t="str">
+        <f>B5</f>
         <v>Ge Chen (Colin)</v>
       </c>
-      <c r="K4" s="16" t="str">
-        <f>J5</f>
+      <c r="L4" s="16" t="str">
+        <f>K5</f>
         <v>Ao Dong</v>
       </c>
-      <c r="L4" s="16" t="str">
-        <f t="shared" ref="L4:L10" si="1">K5</f>
+      <c r="M4" s="16" t="str">
+        <f t="shared" ref="M4:M9" si="0">L5</f>
         <v>Peter Michalski</v>
       </c>
-      <c r="M4" s="13"/>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
-    </row>
-    <row r="5" spans="1:18" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P4" s="13"/>
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
-        <f t="shared" ref="A5:A10" si="2">A4+1</f>
+        <f t="shared" ref="A5:A10" si="1">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -870,39 +910,42 @@
       <c r="C5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="F5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="16"/>
       <c r="I5" s="16"/>
-      <c r="J5" s="16" t="str">
+      <c r="J5" s="16"/>
+      <c r="K5" s="16" t="str">
+        <f>B6</f>
+        <v>Ao Dong</v>
+      </c>
+      <c r="L5" s="16" t="str">
+        <f>K6</f>
+        <v>Peter Michalski</v>
+      </c>
+      <c r="M5" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Ao Dong</v>
-      </c>
-      <c r="K5" s="16" t="str">
-        <f>J6</f>
-        <v>Peter Michalski</v>
-      </c>
-      <c r="L5" s="16" t="str">
-        <f t="shared" si="1"/>
         <v>Sasha Soraine</v>
       </c>
-      <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
-    </row>
-    <row r="6" spans="1:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -911,39 +954,42 @@
       <c r="C6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="F6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="G6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="16"/>
       <c r="I6" s="16"/>
-      <c r="J6" s="16" t="str">
+      <c r="J6" s="16"/>
+      <c r="K6" s="16" t="str">
+        <f>B7</f>
+        <v>Peter Michalski</v>
+      </c>
+      <c r="L6" s="16" t="str">
+        <f>K7</f>
+        <v>Sasha Soraine</v>
+      </c>
+      <c r="M6" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Peter Michalski</v>
-      </c>
-      <c r="K6" s="16" t="str">
-        <f>J7</f>
-        <v>Sasha Soraine</v>
-      </c>
-      <c r="L6" s="16" t="str">
-        <f t="shared" si="1"/>
         <v>Sharon Wu</v>
       </c>
-      <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
-    </row>
-    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P6" s="13"/>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -952,39 +998,42 @@
       <c r="C7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="G7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="H7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="16"/>
       <c r="I7" s="16"/>
-      <c r="J7" s="16" t="str">
+      <c r="J7" s="16"/>
+      <c r="K7" s="16" t="str">
+        <f>B8</f>
+        <v>Sasha Soraine</v>
+      </c>
+      <c r="L7" s="16" t="str">
+        <f>K8</f>
+        <v>Sharon Wu</v>
+      </c>
+      <c r="M7" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Sasha Soraine</v>
-      </c>
-      <c r="K7" s="16" t="str">
-        <f>J8</f>
-        <v>Sharon Wu</v>
-      </c>
-      <c r="L7" s="16" t="str">
-        <f t="shared" si="1"/>
         <v>Zhi Zhang</v>
       </c>
-      <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
-    </row>
-    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P7" s="13"/>
+    </row>
+    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -993,39 +1042,42 @@
       <c r="C8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="G8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="H8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="16"/>
       <c r="I8" s="16"/>
-      <c r="J8" s="16" t="str">
+      <c r="J8" s="16"/>
+      <c r="K8" s="16" t="str">
+        <f>B9</f>
+        <v>Sharon Wu</v>
+      </c>
+      <c r="L8" s="16" t="str">
+        <f>K9</f>
+        <v>Zhi Zhang</v>
+      </c>
+      <c r="M8" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Sharon Wu</v>
-      </c>
-      <c r="K8" s="16" t="str">
-        <f>J9</f>
-        <v>Zhi Zhang</v>
-      </c>
-      <c r="L8" s="16" t="str">
-        <f t="shared" si="1"/>
         <v>Deema Alomair</v>
       </c>
-      <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
-    </row>
-    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P8" s="13"/>
+    </row>
+    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1034,39 +1086,42 @@
       <c r="C9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="16"/>
       <c r="I9" s="16"/>
-      <c r="J9" s="16" t="str">
+      <c r="J9" s="16"/>
+      <c r="K9" s="16" t="str">
+        <f>B10</f>
+        <v>Zhi Zhang</v>
+      </c>
+      <c r="L9" s="16" t="str">
+        <f>K10</f>
+        <v>Deema Alomair</v>
+      </c>
+      <c r="M9" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Zhi Zhang</v>
-      </c>
-      <c r="K9" s="16" t="str">
-        <f>J10</f>
-        <v>Deema Alomair</v>
-      </c>
-      <c r="L9" s="16" t="str">
-        <f t="shared" si="1"/>
         <v>Bo Cao</v>
       </c>
-      <c r="M9" s="13"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
-    </row>
-    <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P9" s="13"/>
+    </row>
+    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1075,42 +1130,45 @@
       <c r="C10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="F10" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="G10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="H10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="16"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="16" t="str">
+      <c r="J10" s="16"/>
+      <c r="K10" s="16" t="str">
         <f>B3</f>
         <v>Deema Alomair</v>
       </c>
-      <c r="K10" s="16" t="str">
-        <f>J3</f>
-        <v>Bo Cao</v>
-      </c>
       <c r="L10" s="16" t="str">
         <f>K3</f>
+        <v>Bo Cao</v>
+      </c>
+      <c r="M10" s="16" t="str">
+        <f>L3</f>
         <v>Ge Chen (Colin)</v>
       </c>
-      <c r="M10" s="13"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
-    </row>
-    <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P10" s="13"/>
+    </row>
+    <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1118,18 +1176,19 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="13"/>
+      <c r="M11" s="4"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
-    </row>
-    <row r="12" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P11" s="13"/>
+    </row>
+    <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1137,17 +1196,18 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="13"/>
+      <c r="M12" s="4"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
-    </row>
-    <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1156,11 +1216,12 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="13"/>
+      <c r="M13" s="4"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
-    </row>
-    <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P13" s="13"/>
+    </row>
+    <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>14</v>
@@ -1175,11 +1236,12 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="13"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
-    </row>
-    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P14" s="13"/>
+    </row>
+    <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1195,11 +1257,12 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15"/>
+      <c r="P15" s="4"/>
       <c r="Q15"/>
       <c r="R15"/>
-    </row>
-    <row r="16" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S15"/>
+    </row>
+    <row r="16" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1218,8 +1281,9 @@
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
-    </row>
-    <row r="17" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S16"/>
+    </row>
+    <row r="17" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1238,8 +1302,9 @@
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17"/>
-    </row>
-    <row r="18" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S17"/>
+    </row>
+    <row r="18" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1258,6 +1323,7 @@
       <c r="P18"/>
       <c r="Q18"/>
       <c r="R18"/>
+      <c r="S18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1269,15 +1335,23 @@
     <hyperlink ref="C7" r:id="rId5" xr:uid="{FDCEAA7B-09B9-394F-9272-06A2E42534F2}"/>
     <hyperlink ref="C8" r:id="rId6" xr:uid="{C907EC9B-B30E-6F49-99C6-F56985FD93FE}"/>
     <hyperlink ref="C10" r:id="rId7" xr:uid="{7253496C-EABA-2645-B050-975DBA0B0108}"/>
-    <hyperlink ref="E3" r:id="rId8" xr:uid="{82DB3A68-C170-F34D-92F3-2B6FA7908C23}"/>
-    <hyperlink ref="E6" r:id="rId9" xr:uid="{9DD92EA4-84F2-1740-8AC0-FA06C087B9A1}"/>
-    <hyperlink ref="E7" r:id="rId10" xr:uid="{953AEC1E-EA56-644B-A121-BE2F1549DE0D}"/>
-    <hyperlink ref="E10" r:id="rId11" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
-    <hyperlink ref="E8" r:id="rId12" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
-    <hyperlink ref="E4" r:id="rId13" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
-    <hyperlink ref="E5" r:id="rId14" xr:uid="{BD77D372-E5FE-7348-A005-C40823ABB1DE}"/>
-    <hyperlink ref="E9" r:id="rId15" xr:uid="{7F6B845B-29C9-EE47-9761-BEFBD243476C}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{82DB3A68-C170-F34D-92F3-2B6FA7908C23}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{9DD92EA4-84F2-1740-8AC0-FA06C087B9A1}"/>
+    <hyperlink ref="F7" r:id="rId10" xr:uid="{953AEC1E-EA56-644B-A121-BE2F1549DE0D}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
+    <hyperlink ref="F8" r:id="rId12" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
+    <hyperlink ref="F5" r:id="rId14" xr:uid="{BD77D372-E5FE-7348-A005-C40823ABB1DE}"/>
+    <hyperlink ref="F9" r:id="rId15" xr:uid="{7F6B845B-29C9-EE47-9761-BEFBD243476C}"/>
     <hyperlink ref="C9" r:id="rId16" xr:uid="{DE229207-DE5E-2148-A086-7C91C16E5E4D}"/>
+    <hyperlink ref="D3" r:id="rId17" display="https://github.com/deemaalomair1" xr:uid="{0F0A777D-DB22-3747-A1C7-415BD42FD85E}"/>
+    <hyperlink ref="D4" r:id="rId18" display="https://github.com/caobo1994" xr:uid="{670FC569-0610-034C-8243-EA06080B4B09}"/>
+    <hyperlink ref="D5" r:id="rId19" display="https://github.com/bigship" xr:uid="{D0DEFFAD-A0C5-F644-AFFD-A0560BDB311D}"/>
+    <hyperlink ref="D6" r:id="rId20" display="https://github.com/Ao99" xr:uid="{1B8F06D6-4598-3D4D-963C-FAECFB4B277F}"/>
+    <hyperlink ref="D7" r:id="rId21" display="https://github.com/peter-michalski" xr:uid="{D0A24253-BB15-DE48-9E16-5D870F79AEF7}"/>
+    <hyperlink ref="D8" r:id="rId22" display="https://github.com/sorainsm" xr:uid="{9A31EA3C-B35B-794E-AC95-BBE4E20880B3}"/>
+    <hyperlink ref="D9" r:id="rId23" display="https://github.com/sharyuwu" xr:uid="{A51DB79D-0D1A-9C4D-B149-C7D25D22A9D6}"/>
+    <hyperlink ref="D10" r:id="rId24" display="https://github.com/best-zhang-zhi" xr:uid="{94F7E293-903D-314C-BEEB-1CD096705463}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Removed unnecessary line in header GitHub ID
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A02154-E211-BC4D-AB59-78669FCE0AAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E231702B-316F-004F-93A3-3D11E06EF463}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -281,7 +281,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -354,6 +354,32 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -386,7 +412,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -418,7 +444,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="23" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="23"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -727,7 +756,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +817,7 @@
       <c r="A2" s="14"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="21"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="7"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>

</xml_diff>

<commit_message>
Update to expert reviewers list
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAAE21A-AC48-B142-9CD9-F2E47C7357FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD1B53A-F728-8C4F-8091-7EF3D9B75370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -762,7 +762,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1009,9 @@
         <v>8</v>
       </c>
       <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="J6" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="K6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Peter Michalski</v>
@@ -1053,7 +1055,9 @@
         <v>40</v>
       </c>
       <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="J7" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Sasha Soraine</v>

</xml_diff>

<commit_message>
Assigned domain experts, all projects approved
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD1B53A-F728-8C4F-8091-7EF3D9B75370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18189D7D-CE25-1F49-80EF-88F5D19A4F68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,18 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$F$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$F$7</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +63,6 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Expert</t>
   </si>
   <si>
@@ -108,9 +111,6 @@
     <t>caob13@mcmaster.ca</t>
   </si>
   <si>
-    <t>cheng54@mcmaster.ca</t>
-  </si>
-  <si>
     <t>donga9@mcmaster.ca</t>
   </si>
   <si>
@@ -138,9 +138,6 @@
     <t>https://github.com/best-zhang-zhi/CAS741Project</t>
   </si>
   <si>
-    <t>Ge Chen (Colin)</t>
-  </si>
-  <si>
     <t>MG + MIS</t>
   </si>
   <si>
@@ -165,18 +162,12 @@
     <t>Fourier Series Library</t>
   </si>
   <si>
-    <t>https://github.com/bigship/CAS741</t>
-  </si>
-  <si>
     <t>Sharon Wu</t>
   </si>
   <si>
     <t>https://github.com/sharyuwu/optimum-tilt-of-solar-panels</t>
   </si>
   <si>
-    <t>HealthyFood</t>
-  </si>
-  <si>
     <t>Double pendulum</t>
   </si>
   <si>
@@ -198,9 +189,6 @@
     <t>caobo1994</t>
   </si>
   <si>
-    <t>bigship</t>
-  </si>
-  <si>
     <t>Ao99</t>
   </si>
   <si>
@@ -216,10 +204,7 @@
     <t>best-zhang-zhi</t>
   </si>
   <si>
-    <t>Ge Chen (Colin)?</t>
-  </si>
-  <si>
-    <t>Deema Alomair?</t>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -759,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,16 +768,16 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>7</v>
@@ -808,10 +793,10 @@
       </c>
       <c r="I1" s="10"/>
       <c r="J1" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L1" s="12"/>
       <c r="M1" s="13"/>
@@ -832,7 +817,7 @@
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>5</v>
@@ -841,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -852,41 +837,41 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="K3" s="16" t="str">
-        <f t="shared" ref="K3:K9" si="0">B4</f>
+        <f t="shared" ref="K3:K8" si="0">B4</f>
         <v>Bo Cao</v>
       </c>
       <c r="L3" s="16" t="str">
         <f>K4</f>
-        <v>Ge Chen (Colin)</v>
+        <v>Ao Dong</v>
       </c>
       <c r="M3" s="16" t="str">
         <f>L4</f>
-        <v>Ao Dong</v>
+        <v>Peter Michalski</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -898,131 +883,133 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="J4" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="K4" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Ge Chen (Colin)</v>
+        <v>Ao Dong</v>
       </c>
       <c r="L4" s="16" t="str">
-        <f t="shared" ref="L4:L9" si="1">K5</f>
-        <v>Ao Dong</v>
+        <f>K5</f>
+        <v>Peter Michalski</v>
       </c>
       <c r="M4" s="16" t="str">
-        <f t="shared" ref="M4:M9" si="2">L5</f>
-        <v>Peter Michalski</v>
+        <f>L5</f>
+        <v>Sasha Soraine</v>
       </c>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
-        <f t="shared" ref="A5:A10" si="3">A4+1</f>
+        <f>A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>55</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="K5" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Ao Dong</v>
+        <v>Peter Michalski</v>
       </c>
       <c r="L5" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Peter Michalski</v>
+        <f t="shared" ref="L5:L8" si="1">K6</f>
+        <v>Sasha Soraine</v>
       </c>
       <c r="M5" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v>Sasha Soraine</v>
+        <f t="shared" ref="M5:M8" si="2">L6</f>
+        <v>Sharon Wu</v>
       </c>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A6:A9" si="3">A5+1</f>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K6" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Peter Michalski</v>
+        <v>Sasha Soraine</v>
       </c>
       <c r="L6" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Sasha Soraine</v>
+        <v>Sharon Wu</v>
       </c>
       <c r="M6" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>Sharon Wu</v>
+        <v>Zhi Zhang</v>
       </c>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
@@ -1037,38 +1024,38 @@
         <v>18</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="16" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Sasha Soraine</v>
+        <v>Sharon Wu</v>
       </c>
       <c r="L7" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Sharon Wu</v>
+        <v>Zhi Zhang</v>
       </c>
       <c r="M7" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>Zhi Zhang</v>
+        <v>Deema Alomair</v>
       </c>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
@@ -1080,39 +1067,41 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="J8" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="K8" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Sharon Wu</v>
+        <v>Zhi Zhang</v>
       </c>
       <c r="L8" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Zhi Zhang</v>
+        <v>Deema Alomair</v>
       </c>
       <c r="M8" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>Deema Alomair</v>
+        <v>Bo Cao</v>
       </c>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
@@ -1124,93 +1113,71 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="J9" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="K9" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Zhi Zhang</v>
+        <f>B3</f>
+        <v>Deema Alomair</v>
       </c>
       <c r="L9" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Deema Alomair</v>
+        <f>K3</f>
+        <v>Bo Cao</v>
       </c>
       <c r="M9" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v>Bo Cao</v>
+        <f>L3</f>
+        <v>Ao Dong</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
     </row>
     <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16" t="str">
-        <f>B3</f>
-        <v>Deema Alomair</v>
-      </c>
-      <c r="L10" s="16" t="str">
-        <f>K3</f>
-        <v>Bo Cao</v>
-      </c>
-      <c r="M10" s="16" t="str">
-        <f>L3</f>
-        <v>Ge Chen (Colin)</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="13"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1231,7 +1198,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1246,11 +1213,11 @@
     </row>
     <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1266,9 +1233,7 @@
     </row>
     <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1280,27 +1245,30 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
     </row>
     <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
       <c r="S15"/>
@@ -1347,54 +1315,30 @@
       <c r="R17"/>
       <c r="S17"/>
     </row>
-    <row r="18" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{EF275338-8768-704D-9514-53651BC63C3E}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{C5C3D4B5-50E6-9044-91CC-55C0D86C8F39}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{5E93B0E7-10BB-964A-95A9-9A15457ACF05}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{99A63936-4E29-9B41-B446-60C325D481D2}"/>
-    <hyperlink ref="C7" r:id="rId5" xr:uid="{FDCEAA7B-09B9-394F-9272-06A2E42534F2}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{C907EC9B-B30E-6F49-99C6-F56985FD93FE}"/>
-    <hyperlink ref="C10" r:id="rId7" xr:uid="{7253496C-EABA-2645-B050-975DBA0B0108}"/>
-    <hyperlink ref="F3" r:id="rId8" xr:uid="{82DB3A68-C170-F34D-92F3-2B6FA7908C23}"/>
-    <hyperlink ref="F6" r:id="rId9" xr:uid="{9DD92EA4-84F2-1740-8AC0-FA06C087B9A1}"/>
-    <hyperlink ref="F7" r:id="rId10" xr:uid="{953AEC1E-EA56-644B-A121-BE2F1549DE0D}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
-    <hyperlink ref="F8" r:id="rId12" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
-    <hyperlink ref="F5" r:id="rId14" xr:uid="{BD77D372-E5FE-7348-A005-C40823ABB1DE}"/>
-    <hyperlink ref="F9" r:id="rId15" xr:uid="{7F6B845B-29C9-EE47-9761-BEFBD243476C}"/>
-    <hyperlink ref="C9" r:id="rId16" xr:uid="{DE229207-DE5E-2148-A086-7C91C16E5E4D}"/>
-    <hyperlink ref="D3" r:id="rId17" display="https://github.com/deemaalomair1" xr:uid="{0F0A777D-DB22-3747-A1C7-415BD42FD85E}"/>
-    <hyperlink ref="D4" r:id="rId18" display="https://github.com/caobo1994" xr:uid="{670FC569-0610-034C-8243-EA06080B4B09}"/>
-    <hyperlink ref="D5" r:id="rId19" display="https://github.com/bigship" xr:uid="{D0DEFFAD-A0C5-F644-AFFD-A0560BDB311D}"/>
-    <hyperlink ref="D6" r:id="rId20" display="https://github.com/Ao99" xr:uid="{1B8F06D6-4598-3D4D-963C-FAECFB4B277F}"/>
-    <hyperlink ref="D7" r:id="rId21" display="https://github.com/peter-michalski" xr:uid="{D0A24253-BB15-DE48-9E16-5D870F79AEF7}"/>
-    <hyperlink ref="D8" r:id="rId22" display="https://github.com/sorainsm" xr:uid="{9A31EA3C-B35B-794E-AC95-BBE4E20880B3}"/>
-    <hyperlink ref="D9" r:id="rId23" display="https://github.com/sharyuwu" xr:uid="{A51DB79D-0D1A-9C4D-B149-C7D25D22A9D6}"/>
-    <hyperlink ref="D10" r:id="rId24" display="https://github.com/best-zhang-zhi" xr:uid="{94F7E293-903D-314C-BEEB-1CD096705463}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{99A63936-4E29-9B41-B446-60C325D481D2}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{FDCEAA7B-09B9-394F-9272-06A2E42534F2}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{C907EC9B-B30E-6F49-99C6-F56985FD93FE}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{7253496C-EABA-2645-B050-975DBA0B0108}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{82DB3A68-C170-F34D-92F3-2B6FA7908C23}"/>
+    <hyperlink ref="F5" r:id="rId8" xr:uid="{9DD92EA4-84F2-1740-8AC0-FA06C087B9A1}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{953AEC1E-EA56-644B-A121-BE2F1549DE0D}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{5E1E8B54-B16A-3845-AC6A-8B21EC5AA5EC}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{51A1721D-3526-3547-A482-74D2BC762D95}"/>
+    <hyperlink ref="F4" r:id="rId12" xr:uid="{DC62EFA2-CDA0-434A-861C-FC54BBC4ACDC}"/>
+    <hyperlink ref="F8" r:id="rId13" xr:uid="{7F6B845B-29C9-EE47-9761-BEFBD243476C}"/>
+    <hyperlink ref="C8" r:id="rId14" xr:uid="{DE229207-DE5E-2148-A086-7C91C16E5E4D}"/>
+    <hyperlink ref="D3" r:id="rId15" display="https://github.com/deemaalomair1" xr:uid="{0F0A777D-DB22-3747-A1C7-415BD42FD85E}"/>
+    <hyperlink ref="D4" r:id="rId16" display="https://github.com/caobo1994" xr:uid="{670FC569-0610-034C-8243-EA06080B4B09}"/>
+    <hyperlink ref="D5" r:id="rId17" display="https://github.com/Ao99" xr:uid="{1B8F06D6-4598-3D4D-963C-FAECFB4B277F}"/>
+    <hyperlink ref="D6" r:id="rId18" display="https://github.com/peter-michalski" xr:uid="{D0A24253-BB15-DE48-9E16-5D870F79AEF7}"/>
+    <hyperlink ref="D7" r:id="rId19" display="https://github.com/sorainsm" xr:uid="{9A31EA3C-B35B-794E-AC95-BBE4E20880B3}"/>
+    <hyperlink ref="D8" r:id="rId20" display="https://github.com/sharyuwu" xr:uid="{A51DB79D-0D1A-9C4D-B149-C7D25D22A9D6}"/>
+    <hyperlink ref="D9" r:id="rId21" display="https://github.com/best-zhang-zhi" xr:uid="{94F7E293-903D-314C-BEEB-1CD096705463}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
SRS Present lecture and updates to Repos.xlsx
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18189D7D-CE25-1F49-80EF-88F5D19A4F68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D823FE75-E17B-D247-9F05-A5D01979F764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="4140" windowWidth="49480" windowHeight="19580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="340" yWindow="14140" windowWidth="50640" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -747,7 +747,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,7 +859,7 @@
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="K3" s="16" t="str">
         <f t="shared" ref="K3:K8" si="0">B4</f>
@@ -951,7 +951,7 @@
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K5" s="16" t="str">
         <f t="shared" si="0"/>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="16" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
@@ -1135,7 +1135,7 @@
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K9" s="16" t="str">
         <f>B3</f>

</xml_diff>

<commit_message>
Domain experts (primary reviewer) shifted so Bo can review double pend, some associated shifts in secondary reviewers
</commit_message>
<xml_diff>
--- a/Repos.xlsx
+++ b/Repos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D823FE75-E17B-D247-9F05-A5D01979F764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646308DF-BEFF-A14B-B912-05606E818277}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="14140" windowWidth="50640" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-600" yWindow="11600" windowWidth="50640" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,10 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$F$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -747,7 +741,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -962,7 +956,7 @@
         <v>Sasha Soraine</v>
       </c>
       <c r="M5" s="16" t="str">
-        <f t="shared" ref="M5:M8" si="2">L6</f>
+        <f>L9</f>
         <v>Sharon Wu</v>
       </c>
       <c r="N5" s="13"/>
@@ -971,7 +965,7 @@
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
-        <f t="shared" ref="A6:A9" si="3">A5+1</f>
+        <f t="shared" ref="A6:A9" si="2">A5+1</f>
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1004,11 +998,11 @@
         <v>Sasha Soraine</v>
       </c>
       <c r="L6" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Sharon Wu</v>
+        <f>K3</f>
+        <v>Bo Cao</v>
       </c>
       <c r="M6" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M5:M8" si="3">L7</f>
         <v>Zhi Zhang</v>
       </c>
       <c r="N6" s="13"/>
@@ -1017,7 +1011,7 @@
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1043,7 +1037,7 @@
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K7" s="16" t="str">
         <f t="shared" si="0"/>
@@ -1054,7 +1048,7 @@
         <v>Zhi Zhang</v>
       </c>
       <c r="M7" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Deema Alomair</v>
       </c>
       <c r="N7" s="13"/>
@@ -1063,7 +1057,7 @@
     </row>
     <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1100,7 +1094,7 @@
         <v>Deema Alomair</v>
       </c>
       <c r="M8" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f>L6</f>
         <v>Bo Cao</v>
       </c>
       <c r="N8" s="13"/>
@@ -1109,7 +1103,7 @@
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1135,15 +1129,15 @@
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K9" s="16" t="str">
         <f>B3</f>
         <v>Deema Alomair</v>
       </c>
       <c r="L9" s="16" t="str">
-        <f>K3</f>
-        <v>Bo Cao</v>
+        <f>K7</f>
+        <v>Sharon Wu</v>
       </c>
       <c r="M9" s="16" t="str">
         <f>L3</f>

</xml_diff>